<commit_message>
updated modles to latest versions
</commit_message>
<xml_diff>
--- a/models/bronchomotor/source/bronchomotor.xlsx
+++ b/models/bronchomotor/source/bronchomotor.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="871">
   <si>
     <t>id</t>
   </si>
@@ -2410,27 +2410,45 @@
     <t>Neuron 1</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-1</t>
+  </si>
+  <si>
     <t>PMID: 8300416, PMID: 3198482, PMID: 2384334</t>
   </si>
   <si>
     <t>Neuron 2</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-2</t>
+  </si>
+  <si>
     <t>doi:10.1016/B978-0-444-53491-0.09985-5</t>
   </si>
   <si>
     <t>Neuron 3</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-3</t>
+  </si>
+  <si>
     <t>Neuron 4</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-4</t>
+  </si>
+  <si>
     <t>Neuron 5</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-5</t>
+  </si>
+  <si>
     <t>Neuron 6</t>
   </si>
   <si>
+    <t>ilxtr:neuron-type-bromo-6</t>
+  </si>
+  <si>
     <t>uri</t>
   </si>
   <si>
@@ -2552,6 +2570,12 @@
   </si>
   <si>
     <t>https://doi.org/</t>
+  </si>
+  <si>
+    <t>ilxtr</t>
+  </si>
+  <si>
+    <t>http://uri.interlex.org/tgbugs/uris/readable/</t>
   </si>
   <si>
     <t>population</t>
@@ -2660,7 +2684,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="28">
+  <fonts count="26">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2745,6 +2769,10 @@
     <font/>
     <font>
       <b/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="&quot;Droid Sans Mono&quot;"/>
     </font>
@@ -2759,29 +2787,11 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <b/>
     </font>
     <font>
       <u/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -2851,7 +2861,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3054,35 +3064,23 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="19" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3092,10 +3090,10 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3400,16 +3398,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>829</v>
+        <v>837</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>830</v>
+        <v>838</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>831</v>
+        <v>839</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>832</v>
+        <v>840</v>
       </c>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
@@ -3424,13 +3422,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>833</v>
+        <v>841</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>834</v>
+        <v>842</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>835</v>
+        <v>843</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -3468,13 +3466,13 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>836</v>
+        <v>844</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>837</v>
+        <v>845</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>838</v>
+        <v>846</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -3490,10 +3488,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>839</v>
+        <v>847</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -3507,10 +3505,10 @@
     <row r="7">
       <c r="A7" s="10"/>
       <c r="B7" s="10" t="s">
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3524,10 +3522,10 @@
     <row r="8">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
-        <v>842</v>
+        <v>850</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3541,10 +3539,10 @@
     <row r="9">
       <c r="A9" s="10"/>
       <c r="B9" s="10" t="s">
-        <v>843</v>
+        <v>851</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3570,10 +3568,10 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>844</v>
+        <v>852</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3587,10 +3585,10 @@
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="B12" s="79" t="s">
-        <v>847</v>
+        <v>854</v>
+      </c>
+      <c r="B12" s="77" t="s">
+        <v>855</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -3604,10 +3602,10 @@
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>848</v>
-      </c>
-      <c r="B13" s="79" t="s">
-        <v>849</v>
+        <v>856</v>
+      </c>
+      <c r="B13" s="77" t="s">
+        <v>857</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3634,10 +3632,10 @@
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>850</v>
-      </c>
-      <c r="B15" s="80" t="s">
-        <v>851</v>
+        <v>858</v>
+      </c>
+      <c r="B15" s="78" t="s">
+        <v>859</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -3651,27 +3649,27 @@
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="B16" s="81" t="s">
+        <v>860</v>
+      </c>
+      <c r="B16" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>853</v>
-      </c>
-      <c r="B17" s="81" t="s">
-        <v>854</v>
+        <v>861</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>862</v>
       </c>
     </row>
     <row r="18">
@@ -3693,46 +3691,46 @@
       <c r="A23" s="10"/>
     </row>
     <row r="24">
-      <c r="A24" s="68" t="s">
-        <v>855</v>
-      </c>
-      <c r="B24" s="82" t="s">
-        <v>856</v>
+      <c r="A24" s="69" t="s">
+        <v>863</v>
+      </c>
+      <c r="B24" s="80" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="68" t="s">
-        <v>857</v>
-      </c>
-      <c r="B25" s="82" t="s">
-        <v>858</v>
+      <c r="A25" s="69" t="s">
+        <v>865</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>866</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="68" t="s">
-        <v>859</v>
-      </c>
-      <c r="B26" s="83" t="s">
-        <v>860</v>
-      </c>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
+      <c r="A26" s="69" t="s">
+        <v>867</v>
+      </c>
+      <c r="B26" s="81" t="s">
+        <v>868</v>
+      </c>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
     </row>
     <row r="27" hidden="1">
       <c r="A27" s="10" t="s">
-        <v>861</v>
+        <v>869</v>
       </c>
     </row>
     <row r="28" hidden="1">
       <c r="A28" s="10" t="s">
-        <v>862</v>
+        <v>870</v>
       </c>
     </row>
     <row r="29">
@@ -8357,9 +8355,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="28.57"/>
-    <col customWidth="1" min="5" max="5" width="34.14"/>
-    <col customWidth="1" min="7" max="7" width="46.57"/>
+    <col customWidth="1" min="3" max="3" width="21.71"/>
+    <col customWidth="1" min="5" max="5" width="28.57"/>
+    <col customWidth="1" min="6" max="6" width="34.14"/>
+    <col customWidth="1" min="8" max="8" width="46.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8369,40 +8368,24 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>632</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="E1" s="61" t="s">
         <v>777</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="F1" s="61" t="s">
         <v>778</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>779</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>574</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
@@ -8411,9 +8394,12 @@
       <c r="B2" s="4" t="s">
         <v>780</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>781</v>
+      </c>
+      <c r="F2" s="67"/>
+      <c r="H2" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="3">
@@ -8421,11 +8407,14 @@
         <v>412</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>782</v>
-      </c>
-      <c r="E3" s="67"/>
-      <c r="G3" s="4" t="s">
         <v>783</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>784</v>
+      </c>
+      <c r="F3" s="67"/>
+      <c r="H3" s="4" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="4">
@@ -8433,11 +8422,14 @@
         <v>415</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="E4" s="67"/>
-      <c r="G4" s="4" t="s">
-        <v>783</v>
+        <v>786</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>787</v>
+      </c>
+      <c r="F4" s="67"/>
+      <c r="H4" s="4" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="5">
@@ -8445,11 +8437,14 @@
         <v>418</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>789</v>
+      </c>
+      <c r="F5" s="67"/>
+      <c r="H5" s="4" t="s">
         <v>785</v>
-      </c>
-      <c r="E5" s="67"/>
-      <c r="G5" s="4" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="6">
@@ -8457,11 +8452,14 @@
         <v>421</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>786</v>
-      </c>
-      <c r="E6" s="67"/>
-      <c r="G6" s="4" t="s">
-        <v>783</v>
+        <v>790</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>791</v>
+      </c>
+      <c r="F6" s="67"/>
+      <c r="H6" s="4" t="s">
+        <v>785</v>
       </c>
     </row>
     <row r="7">
@@ -8469,11 +8467,14 @@
         <v>424</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>787</v>
-      </c>
-      <c r="E7" s="67"/>
-      <c r="G7" s="4" t="s">
-        <v>783</v>
+        <v>792</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>793</v>
+      </c>
+      <c r="F7" s="67"/>
+      <c r="H7" s="4" t="s">
+        <v>785</v>
       </c>
     </row>
   </sheetData>
@@ -8496,66 +8497,66 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>788</v>
+        <v>794</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>790</v>
-      </c>
-      <c r="C2" s="70" t="s">
-        <v>791</v>
+        <v>796</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>792</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>793</v>
+        <v>798</v>
+      </c>
+      <c r="C3" s="71" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>794</v>
-      </c>
-      <c r="C4" s="70" t="s">
-        <v>795</v>
+        <v>800</v>
+      </c>
+      <c r="C4" s="71" t="s">
+        <v>801</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>796</v>
-      </c>
-      <c r="C5" s="70" t="s">
-        <v>797</v>
+        <v>802</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>783</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>798</v>
-      </c>
-      <c r="D6" s="72"/>
+        <v>785</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>804</v>
+      </c>
+      <c r="D6" s="73"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>799</v>
-      </c>
-      <c r="C7" s="71" t="s">
-        <v>800</v>
+        <v>805</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>806</v>
       </c>
     </row>
   </sheetData>
@@ -8577,452 +8578,124 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="73" t="s">
-        <v>801</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>802</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
+      <c r="A1" s="74" t="s">
+        <v>807</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
-        <v>803</v>
-      </c>
-      <c r="B2" s="74" t="s">
-        <v>804</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
+      <c r="A2" s="75" t="s">
+        <v>809</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>805</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>806</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
+      <c r="A3" s="75" t="s">
+        <v>811</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>807</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>808</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
+      <c r="A4" s="75" t="s">
+        <v>813</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="14" t="s">
-        <v>809</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>810</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
+      <c r="A5" s="75" t="s">
+        <v>815</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="s">
-        <v>811</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>812</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
+      <c r="A6" s="75" t="s">
+        <v>817</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>813</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>814</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="Z7" s="10"/>
+      <c r="A7" s="75" t="s">
+        <v>819</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>815</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>816</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
+      <c r="A8" s="75" t="s">
+        <v>821</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>817</v>
-      </c>
-      <c r="B9" s="75" t="s">
-        <v>818</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
+      <c r="A9" s="75" t="s">
+        <v>823</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="14" t="s">
-        <v>819</v>
-      </c>
-      <c r="B10" s="75" t="s">
-        <v>820</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
+      <c r="A10" s="75" t="s">
+        <v>825</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="14" t="s">
-        <v>821</v>
-      </c>
-      <c r="B11" s="75" t="s">
-        <v>822</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="10"/>
+      <c r="A11" s="75" t="s">
+        <v>827</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>823</v>
+      <c r="A12" s="75" t="s">
+        <v>829</v>
       </c>
       <c r="B12" s="76" t="s">
-        <v>824</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
+        <v>830</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="35" t="s">
-        <v>825</v>
-      </c>
-      <c r="B13" s="77" t="s">
-        <v>826</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="10"/>
+      <c r="A13" s="75" t="s">
+        <v>831</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>827</v>
-      </c>
-      <c r="B14" s="78" t="s">
-        <v>828</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="10"/>
+      <c r="A14" s="75" t="s">
+        <v>833</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="75" t="s">
+        <v>835</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>836</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9039,7 +8712,8 @@
     <hyperlink r:id="rId11" ref="B12"/>
     <hyperlink r:id="rId12" ref="B13"/>
     <hyperlink r:id="rId13" ref="B14"/>
+    <hyperlink r:id="rId14" ref="B15"/>
   </hyperlinks>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes from apinat-build --all for 2022-07-19T0344Z
synchronize latest changes via apinat-build
</commit_message>
<xml_diff>
--- a/models/bronchomotor/source/bronchomotor.xlsx
+++ b/models/bronchomotor/source/bronchomotor.xlsx
@@ -1112,7 +1112,7 @@
     <t>B102</t>
   </si>
   <si>
-    <t>terminal bronchiole</t>
+    <t>Terminal bronchiole</t>
   </si>
   <si>
     <t>UBERON:0002187</t>
@@ -1130,7 +1130,7 @@
     <t>B103</t>
   </si>
   <si>
-    <t>bronchiole</t>
+    <t>Bronchiole</t>
   </si>
   <si>
     <t>UBERON:0002186</t>
@@ -1145,7 +1145,7 @@
     <t>B104</t>
   </si>
   <si>
-    <t>bronchus</t>
+    <t>Bronchus</t>
   </si>
   <si>
     <t>UBERON:0002185</t>
@@ -1160,7 +1160,7 @@
     <t>B105</t>
   </si>
   <si>
-    <t>trachea</t>
+    <t>Trachea</t>
   </si>
   <si>
     <t>UBERON:0003126</t>
@@ -1232,7 +1232,7 @@
     <t>B119</t>
   </si>
   <si>
-    <t>trachea parasympathetic ganglia</t>
+    <t>Trachea parasympathetic ganglia</t>
   </si>
   <si>
     <t>NCIT:C52557</t>
@@ -1241,19 +1241,19 @@
     <t>B120</t>
   </si>
   <si>
-    <t>bronchus parasympathetic ganglia</t>
+    <t>Bronchus parasympathetic ganglia</t>
   </si>
   <si>
     <t>B121</t>
   </si>
   <si>
-    <t>bronchiole parasympathetic ganglia</t>
+    <t>Bronchiole parasympathetic ganglia</t>
   </si>
   <si>
     <t>B122</t>
   </si>
   <si>
-    <t>terminal bronchiole parasympathetic ganglia</t>
+    <t>Terminal bronchiole parasympathetic ganglia</t>
   </si>
   <si>
     <t>B123</t>

</xml_diff>

<commit_message>
update sstom aacar bromo
aacar fix housing lyph inversion affecting aacar-6, remove spurious
layer from aacar-11

bromo fix duplicate id issue between T11gr and T12gr

sstom remove axon going to mucosa from sstom-13 (see discussion on npo
vs apinat modelling on this one, it is not so simple)
</commit_message>
<xml_diff>
--- a/models/bronchomotor/source/bronchomotor.xlsx
+++ b/models/bronchomotor/source/bronchomotor.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="941">
   <si>
     <t>id</t>
   </si>
@@ -1061,7 +1061,10 @@
     <t>B96</t>
   </si>
   <si>
-    <t>T12 ray ramus</t>
+    <t>ILX:0739298</t>
+  </si>
+  <si>
+    <t>T12 gray ramus</t>
   </si>
   <si>
     <t>B97</t>
@@ -1136,7 +1139,7 @@
     <t>B117, B122, B118</t>
   </si>
   <si>
-    <t>0,0,0,0</t>
+    <t>1,1,1</t>
   </si>
   <si>
     <t>B103</t>
@@ -3124,7 +3127,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3317,6 +3320,16 @@
     </xf>
     <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -3746,48 +3759,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="105" t="s">
-        <v>902</v>
-      </c>
-      <c r="B2" s="106" t="s">
+      <c r="A2" s="109" t="s">
         <v>903</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="B2" s="110" t="s">
         <v>904</v>
       </c>
+      <c r="C2" s="111" t="s">
+        <v>905</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="105" t="s">
+      <c r="A3" s="109" t="s">
+        <v>906</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="C3" s="111" t="s">
         <v>905</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>906</v>
-      </c>
-      <c r="C3" s="107" t="s">
-        <v>904</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="105" t="s">
-        <v>907</v>
+      <c r="A4" s="109" t="s">
+        <v>908</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>908</v>
-      </c>
-      <c r="C4" s="107" t="s">
-        <v>904</v>
+        <v>909</v>
+      </c>
+      <c r="C4" s="111" t="s">
+        <v>905</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="107" t="s">
-        <v>909</v>
-      </c>
-      <c r="C5" s="107" t="s">
-        <v>904</v>
+      <c r="B5" s="111" t="s">
+        <v>910</v>
+      </c>
+      <c r="C5" s="111" t="s">
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -3814,123 +3827,123 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="108" t="s">
-        <v>910</v>
-      </c>
-      <c r="B1" s="108" t="s">
+      <c r="A1" s="112" t="s">
         <v>911</v>
+      </c>
+      <c r="B1" s="112" t="s">
+        <v>912</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>912</v>
-      </c>
-      <c r="B2" s="109" t="s">
         <v>913</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31" t="s">
-        <v>914</v>
-      </c>
-      <c r="B3" s="109" t="s">
         <v>915</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>916</v>
-      </c>
-      <c r="B4" s="109" t="s">
         <v>917</v>
+      </c>
+      <c r="B4" s="113" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>918</v>
-      </c>
-      <c r="B5" s="109" t="s">
         <v>919</v>
+      </c>
+      <c r="B5" s="113" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>920</v>
-      </c>
-      <c r="B6" s="109" t="s">
         <v>921</v>
+      </c>
+      <c r="B6" s="113" t="s">
+        <v>922</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>922</v>
-      </c>
-      <c r="B7" s="109" t="s">
         <v>923</v>
+      </c>
+      <c r="B7" s="113" t="s">
+        <v>924</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>924</v>
-      </c>
-      <c r="B8" s="109" t="s">
         <v>925</v>
+      </c>
+      <c r="B8" s="113" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>926</v>
-      </c>
-      <c r="B9" s="109" t="s">
         <v>927</v>
+      </c>
+      <c r="B9" s="113" t="s">
+        <v>928</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>928</v>
-      </c>
-      <c r="B10" s="109" t="s">
         <v>929</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>930</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="31" t="s">
-        <v>930</v>
-      </c>
-      <c r="B11" s="109" t="s">
         <v>931</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="31" t="s">
-        <v>932</v>
-      </c>
-      <c r="B12" s="109" t="s">
         <v>933</v>
+      </c>
+      <c r="B12" s="113" t="s">
+        <v>934</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="31" t="s">
-        <v>934</v>
-      </c>
-      <c r="B13" s="109" t="s">
         <v>935</v>
+      </c>
+      <c r="B13" s="113" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="31" t="s">
-        <v>936</v>
-      </c>
-      <c r="B14" s="109" t="s">
         <v>937</v>
+      </c>
+      <c r="B14" s="113" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="31" t="s">
-        <v>938</v>
-      </c>
-      <c r="B15" s="109" t="s">
         <v>939</v>
+      </c>
+      <c r="B15" s="113" t="s">
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -3970,7 +3983,7 @@
     <col customWidth="1" min="2" max="2" width="14.75"/>
     <col customWidth="1" min="3" max="3" width="22.38"/>
     <col customWidth="1" min="13" max="13" width="26.88"/>
-    <col customWidth="1" min="14" max="14" width="16.75"/>
+    <col customWidth="1" min="14" max="14" width="20.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4358,7 +4371,7 @@
         <v>86</v>
       </c>
       <c r="N17" s="5">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="18">
@@ -5339,77 +5352,77 @@
       <c r="A99" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="B99" s="28" t="s">
-        <v>328</v>
+      <c r="B99" s="31" t="s">
+        <v>331</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="I99" s="11"/>
     </row>
     <row r="100">
       <c r="A100" s="12" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I100" s="11"/>
     </row>
     <row r="101">
       <c r="A101" s="12" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="I101" s="4"/>
     </row>
     <row r="102">
       <c r="A102" s="12" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="15" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B103" s="37" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="I103" s="11"/>
     </row>
     <row r="104">
       <c r="A104" s="12" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B104" s="37" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="I104" s="4"/>
       <c r="M104" s="5" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N104" s="5">
         <v>0.0</v>
@@ -5417,24 +5430,24 @@
     </row>
     <row r="105">
       <c r="A105" s="15" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B105" s="37" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="38" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B106" s="39" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C106" s="40" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D106" s="41"/>
       <c r="E106" s="41"/>
@@ -5442,16 +5455,16 @@
       <c r="G106" s="41"/>
       <c r="H106" s="41"/>
       <c r="I106" s="42" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="J106" s="41"/>
       <c r="K106" s="41"/>
       <c r="L106" s="41"/>
       <c r="M106" s="40" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="N106" s="40" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O106" s="41"/>
       <c r="P106" s="41"/>
@@ -5460,13 +5473,13 @@
     </row>
     <row r="107">
       <c r="A107" s="43" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B107" s="39" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C107" s="40" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D107" s="41"/>
       <c r="E107" s="41"/>
@@ -5474,16 +5487,16 @@
       <c r="G107" s="41"/>
       <c r="H107" s="41"/>
       <c r="I107" s="42" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="J107" s="41"/>
       <c r="K107" s="41"/>
       <c r="L107" s="41"/>
       <c r="M107" s="40" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="N107" s="40" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O107" s="41"/>
       <c r="P107" s="41"/>
@@ -5492,13 +5505,13 @@
     </row>
     <row r="108">
       <c r="A108" s="43" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B108" s="44" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C108" s="40" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D108" s="41"/>
       <c r="E108" s="41"/>
@@ -5506,16 +5519,16 @@
       <c r="G108" s="41"/>
       <c r="H108" s="41"/>
       <c r="I108" s="42" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="J108" s="41"/>
       <c r="K108" s="41"/>
       <c r="L108" s="41"/>
       <c r="M108" s="40" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N108" s="40" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O108" s="41"/>
       <c r="P108" s="41"/>
@@ -5524,13 +5537,13 @@
     </row>
     <row r="109">
       <c r="A109" s="38" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B109" s="44" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C109" s="40" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D109" s="41"/>
       <c r="E109" s="41"/>
@@ -5538,16 +5551,16 @@
       <c r="G109" s="41"/>
       <c r="H109" s="41"/>
       <c r="I109" s="42" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="J109" s="41"/>
       <c r="K109" s="41"/>
       <c r="L109" s="41"/>
       <c r="M109" s="40" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N109" s="40" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="O109" s="41"/>
       <c r="P109" s="41"/>
@@ -5556,153 +5569,153 @@
     </row>
     <row r="110">
       <c r="A110" s="15" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B110" s="45" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I110" s="11"/>
     </row>
     <row r="111">
       <c r="A111" s="15" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B111" s="37" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="I111" s="11"/>
     </row>
     <row r="112">
       <c r="A112" s="12" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B112" s="37" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="I112" s="11"/>
     </row>
     <row r="113">
       <c r="A113" s="12" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B113" s="37" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I113" s="11"/>
     </row>
     <row r="114">
       <c r="A114" s="15" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B114" s="37" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E114" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="15" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B115" s="37" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E115" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I115" s="24"/>
       <c r="M115" s="5" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="15" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B116" s="46" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I116" s="24"/>
       <c r="M116" s="47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="15" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B117" s="46" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I117" s="24"/>
       <c r="M117" s="47" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="15" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B118" s="46" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I118" s="24"/>
       <c r="M118" s="47" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="15" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B119" s="46" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I119" s="24"/>
       <c r="M119" s="47" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="15" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B120" s="26" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>173</v>
@@ -5711,163 +5724,163 @@
     </row>
     <row r="121">
       <c r="A121" s="15" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B121" s="37" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C121" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I121" s="24"/>
     </row>
     <row r="122">
       <c r="A122" s="12" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B122" s="37" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I122" s="24"/>
     </row>
     <row r="123">
       <c r="A123" s="12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B123" s="37" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="I123" s="24"/>
     </row>
     <row r="124">
       <c r="A124" s="15" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B124" s="37" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I124" s="11"/>
     </row>
     <row r="125">
       <c r="A125" s="12" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B125" s="37" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="I125" s="24"/>
     </row>
     <row r="126">
       <c r="A126" s="15" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B126" s="37" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I126" s="11"/>
     </row>
     <row r="127">
       <c r="A127" s="15" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B127" s="37" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="I127" s="11"/>
     </row>
     <row r="128">
       <c r="A128" s="12" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B128" s="37" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="I128" s="11"/>
     </row>
     <row r="129">
       <c r="A129" s="12" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B129" s="37" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C129" s="48" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I129" s="11"/>
     </row>
     <row r="130">
       <c r="A130" s="49" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E130" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I130" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="50" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E131" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I131" s="11"/>
     </row>
     <row r="132">
       <c r="A132" s="51" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B132" s="52" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C132" s="53" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D132" s="11"/>
       <c r="E132" s="54" t="b">
         <v>1</v>
       </c>
       <c r="F132" s="26" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
@@ -5884,20 +5897,20 @@
     </row>
     <row r="133">
       <c r="A133" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B133" s="52" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C133" s="53" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D133" s="11"/>
       <c r="E133" s="54" t="b">
         <v>1</v>
       </c>
       <c r="F133" s="26" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
@@ -5914,20 +5927,20 @@
     </row>
     <row r="134">
       <c r="A134" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B134" s="52" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C134" s="53" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D134" s="11"/>
       <c r="E134" s="54" t="b">
         <v>1</v>
       </c>
       <c r="F134" s="26" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
@@ -5944,20 +5957,20 @@
     </row>
     <row r="135">
       <c r="A135" s="51" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B135" s="52" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C135" s="53" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D135" s="11"/>
       <c r="E135" s="54" t="b">
         <v>1</v>
       </c>
       <c r="F135" s="26" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
@@ -5977,20 +5990,20 @@
         <v>26</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I136" s="11"/>
       <c r="J136" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R136" s="5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="137">
@@ -5998,17 +6011,17 @@
         <v>30</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I137" s="11"/>
       <c r="J137" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="138">
@@ -6016,17 +6029,17 @@
         <v>34</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I138" s="11"/>
       <c r="J138" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="139">
@@ -6034,17 +6047,17 @@
         <v>38</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I139" s="11"/>
       <c r="J139" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="140">
@@ -6052,17 +6065,17 @@
         <v>42</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I140" s="11"/>
       <c r="J140" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="141">
@@ -6070,17 +6083,17 @@
         <v>46</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I141" s="11"/>
       <c r="J141" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="142">
@@ -6088,17 +6101,17 @@
         <v>50</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I142" s="11"/>
       <c r="J142" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="143">
@@ -6106,17 +6119,17 @@
         <v>54</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I143" s="11"/>
       <c r="J143" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="144">
@@ -6124,17 +6137,17 @@
         <v>58</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I144" s="11"/>
       <c r="J144" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="145">
@@ -6142,17 +6155,17 @@
         <v>62</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F145" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I145" s="11"/>
       <c r="J145" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="146">
@@ -6160,17 +6173,17 @@
         <v>66</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I146" s="11"/>
       <c r="J146" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="147">
@@ -6178,17 +6191,17 @@
         <v>70</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F147" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I147" s="11"/>
       <c r="J147" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="148">
@@ -6196,17 +6209,17 @@
         <v>74</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I148" s="11"/>
       <c r="J148" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="149">
@@ -6214,17 +6227,17 @@
         <v>78</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F149" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I149" s="11"/>
       <c r="J149" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="150">
@@ -6232,104 +6245,104 @@
         <v>89</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="F150" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I150" s="11"/>
       <c r="J150" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R150" s="5" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F151" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I151" s="11"/>
       <c r="J151" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R151" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I152" s="11"/>
       <c r="J152" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R152" s="5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="F153" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I153" s="11"/>
       <c r="J153" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R153" s="5" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I154" s="11"/>
       <c r="J154" s="5" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R154" s="5" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="155">
@@ -6337,10 +6350,10 @@
         <v>229.0</v>
       </c>
       <c r="B155" s="52" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C155" s="53" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="57" t="b">
@@ -6350,7 +6363,7 @@
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
       <c r="I155" s="58" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="J155" s="53"/>
       <c r="K155" s="58"/>
@@ -6405,52 +6418,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="J1" s="61" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="L1" s="62" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="K2" s="65">
         <v>6.0</v>
@@ -6461,46 +6474,46 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K3" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L3" s="65" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="K4" s="65">
         <v>6.0</v>
@@ -6511,45 +6524,45 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E5" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K5" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L5" s="65" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="K6" s="65">
         <v>6.0</v>
@@ -6560,45 +6573,45 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K7" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L7" s="65" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="K8" s="65">
         <v>6.0</v>
@@ -6609,45 +6622,45 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K9" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L9" s="65" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E10" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="K10" s="65">
         <v>6.0</v>
@@ -6658,45 +6671,45 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E11" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L11" s="65" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E12" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="K12" s="65">
         <v>6.0</v>
@@ -6707,45 +6720,45 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K13" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L13" s="65" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E14" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="K14" s="65">
         <v>6.0</v>
@@ -6756,45 +6769,45 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K15" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L15" s="65" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K16" s="65">
         <v>6.0</v>
@@ -6805,45 +6818,45 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K17" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L17" s="65" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="K18" s="65">
         <v>6.0</v>
@@ -6854,45 +6867,45 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E19" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K19" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L19" s="65" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E20" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="K20" s="65">
         <v>6.0</v>
@@ -6903,144 +6916,165 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E21" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K21" s="65" t="s">
+        <v>499</v>
+      </c>
+      <c r="L21" s="65" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="66" t="s">
+        <v>564</v>
+      </c>
+      <c r="B22" s="67" t="s">
+        <v>565</v>
+      </c>
+      <c r="C22" s="68" t="s">
+        <v>492</v>
+      </c>
+      <c r="D22" s="69"/>
+      <c r="E22" s="70" t="s">
+        <v>449</v>
+      </c>
+      <c r="F22" s="66" t="s">
+        <v>566</v>
+      </c>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="66">
+        <v>6.0</v>
+      </c>
+      <c r="L22" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="69"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="66" t="s">
+        <v>567</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>568</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>496</v>
+      </c>
+      <c r="D23" s="69"/>
+      <c r="E23" s="70" t="s">
+        <v>446</v>
+      </c>
+      <c r="F23" s="66" t="s">
+        <v>569</v>
+      </c>
+      <c r="G23" s="66" t="s">
         <v>498</v>
       </c>
-      <c r="L21" s="65" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>563</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>564</v>
-      </c>
-      <c r="C22" s="63" t="s">
-        <v>491</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>448</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>565</v>
-      </c>
-      <c r="K22" s="65">
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="66" t="s">
+        <v>499</v>
+      </c>
+      <c r="L23" s="66" t="s">
+        <v>570</v>
+      </c>
+      <c r="M23" s="69"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="66" t="s">
+        <v>571</v>
+      </c>
+      <c r="B24" s="67" t="s">
+        <v>572</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>492</v>
+      </c>
+      <c r="D24" s="69"/>
+      <c r="E24" s="70" t="s">
+        <v>449</v>
+      </c>
+      <c r="F24" s="66" t="s">
+        <v>573</v>
+      </c>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="66"/>
+      <c r="K24" s="66">
         <v>6.0</v>
       </c>
-      <c r="L22" s="65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>567</v>
-      </c>
-      <c r="C23" s="63" t="s">
-        <v>495</v>
-      </c>
-      <c r="E23" s="51" t="s">
-        <v>445</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="K23" s="65" t="s">
+      <c r="L24" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="69"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="66" t="s">
+        <v>574</v>
+      </c>
+      <c r="B25" s="67" t="s">
+        <v>575</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>496</v>
+      </c>
+      <c r="D25" s="69"/>
+      <c r="E25" s="70" t="s">
+        <v>446</v>
+      </c>
+      <c r="F25" s="66" t="s">
+        <v>576</v>
+      </c>
+      <c r="G25" s="66" t="s">
         <v>498</v>
       </c>
-      <c r="L23" s="65" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="5" t="s">
-        <v>570</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>571</v>
-      </c>
-      <c r="C24" s="63" t="s">
-        <v>491</v>
-      </c>
-      <c r="E24" s="51" t="s">
-        <v>448</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="J24" s="65"/>
-      <c r="K24" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="L24" s="65" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>573</v>
-      </c>
-      <c r="B25" s="37" t="s">
-        <v>574</v>
-      </c>
-      <c r="C25" s="63" t="s">
-        <v>495</v>
-      </c>
-      <c r="E25" s="51" t="s">
-        <v>445</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>497</v>
-      </c>
-      <c r="K25" s="65" t="s">
-        <v>498</v>
-      </c>
-      <c r="L25" s="65" t="s">
-        <v>576</v>
-      </c>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="66" t="s">
+        <v>499</v>
+      </c>
+      <c r="L25" s="66" t="s">
+        <v>577</v>
+      </c>
+      <c r="M25" s="69"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="K26" s="65">
         <v>6.0</v>
@@ -7051,45 +7085,45 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K27" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L27" s="65" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E28" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="K28" s="65">
         <v>6.0</v>
@@ -7100,72 +7134,72 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K29" s="65" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L29" s="65" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="K30" s="66" t="s">
-        <v>594</v>
-      </c>
-      <c r="L30" s="67" t="s">
         <v>595</v>
+      </c>
+      <c r="L30" s="71" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="40" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>597</v>
-      </c>
-      <c r="C31" s="68" t="s">
-        <v>491</v>
+        <v>598</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>492</v>
       </c>
       <c r="D31" s="41"/>
-      <c r="E31" s="69" t="s">
-        <v>448</v>
+      <c r="E31" s="73" t="s">
+        <v>449</v>
       </c>
       <c r="F31" s="40" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
@@ -7181,224 +7215,224 @@
     </row>
     <row r="32">
       <c r="A32" s="40" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>600</v>
-      </c>
-      <c r="C32" s="68" t="s">
-        <v>495</v>
+        <v>601</v>
+      </c>
+      <c r="C32" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D32" s="41"/>
-      <c r="E32" s="69" t="s">
-        <v>445</v>
+      <c r="E32" s="73" t="s">
+        <v>446</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="G32" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="H32" s="41"/>
       <c r="I32" s="41"/>
       <c r="J32" s="41"/>
       <c r="K32" s="66" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="L32" s="40" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="M32" s="41"/>
     </row>
     <row r="33">
       <c r="A33" s="40" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>606</v>
-      </c>
-      <c r="C33" s="68" t="s">
-        <v>495</v>
+        <v>607</v>
+      </c>
+      <c r="C33" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D33" s="41"/>
-      <c r="E33" s="69" t="s">
-        <v>441</v>
+      <c r="E33" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F33" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G33" s="40" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
       <c r="J33" s="41"/>
       <c r="K33" s="66" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L33" s="40" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="M33" s="41"/>
     </row>
     <row r="34">
       <c r="A34" s="40" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>610</v>
-      </c>
-      <c r="C34" s="68" t="s">
-        <v>495</v>
+        <v>611</v>
+      </c>
+      <c r="C34" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D34" s="41"/>
-      <c r="E34" s="69" t="s">
-        <v>441</v>
+      <c r="E34" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F34" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G34" s="40" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="H34" s="41"/>
       <c r="I34" s="41"/>
       <c r="J34" s="41"/>
       <c r="K34" s="66" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L34" s="40" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="M34" s="41"/>
     </row>
     <row r="35">
       <c r="A35" s="40" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>614</v>
-      </c>
-      <c r="C35" s="68" t="s">
-        <v>495</v>
+        <v>615</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D35" s="41"/>
-      <c r="E35" s="69" t="s">
-        <v>441</v>
+      <c r="E35" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F35" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G35" s="40" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="H35" s="41"/>
       <c r="I35" s="41"/>
       <c r="J35" s="41"/>
       <c r="K35" s="66" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L35" s="40" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="M35" s="41"/>
     </row>
     <row r="36">
       <c r="A36" s="40" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>618</v>
-      </c>
-      <c r="C36" s="68" t="s">
-        <v>495</v>
+        <v>619</v>
+      </c>
+      <c r="C36" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D36" s="41"/>
-      <c r="E36" s="69" t="s">
-        <v>441</v>
+      <c r="E36" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F36" s="40" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="G36" s="40" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H36" s="41"/>
       <c r="I36" s="41"/>
       <c r="J36" s="41"/>
       <c r="K36" s="66" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="L36" s="40" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="M36" s="41"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E37" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="K37" s="5">
         <v>0.0</v>
       </c>
       <c r="L37" s="5" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="K38" s="66" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L38" s="5" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="40" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>631</v>
-      </c>
-      <c r="C39" s="68" t="s">
-        <v>491</v>
+        <v>632</v>
+      </c>
+      <c r="C39" s="72" t="s">
+        <v>492</v>
       </c>
       <c r="D39" s="41"/>
-      <c r="E39" s="69" t="s">
-        <v>448</v>
+      <c r="E39" s="73" t="s">
+        <v>449</v>
       </c>
       <c r="F39" s="40" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="G39" s="41"/>
       <c r="H39" s="41"/>
@@ -7408,106 +7442,106 @@
         <v>0.0</v>
       </c>
       <c r="L39" s="40" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M39" s="41"/>
     </row>
     <row r="40">
       <c r="A40" s="40" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>634</v>
-      </c>
-      <c r="C40" s="68" t="s">
-        <v>495</v>
+        <v>635</v>
+      </c>
+      <c r="C40" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D40" s="41"/>
-      <c r="E40" s="69" t="s">
-        <v>441</v>
+      <c r="E40" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="H40" s="41"/>
       <c r="I40" s="41"/>
       <c r="J40" s="41"/>
       <c r="K40" s="66" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L40" s="40" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="M40" s="41"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E41" s="51" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="K41" s="5">
         <v>0.0</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E42" s="51" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="K42" s="66" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L42" s="5" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="40" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>647</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>491</v>
+        <v>648</v>
+      </c>
+      <c r="C43" s="72" t="s">
+        <v>492</v>
       </c>
       <c r="D43" s="41"/>
-      <c r="E43" s="69" t="s">
-        <v>448</v>
+      <c r="E43" s="73" t="s">
+        <v>449</v>
       </c>
       <c r="F43" s="40" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="G43" s="41"/>
       <c r="H43" s="41"/>
@@ -7517,60 +7551,60 @@
         <v>0.0</v>
       </c>
       <c r="L43" s="40" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M43" s="41"/>
     </row>
     <row r="44">
       <c r="A44" s="40" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>650</v>
-      </c>
-      <c r="C44" s="68" t="s">
-        <v>495</v>
+        <v>651</v>
+      </c>
+      <c r="C44" s="72" t="s">
+        <v>496</v>
       </c>
       <c r="D44" s="41"/>
-      <c r="E44" s="69" t="s">
-        <v>441</v>
+      <c r="E44" s="73" t="s">
+        <v>442</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="H44" s="41"/>
       <c r="I44" s="41"/>
       <c r="J44" s="41"/>
       <c r="K44" s="66" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="L44" s="40" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="M44" s="41"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="D45" s="70" t="s">
         <v>657</v>
+      </c>
+      <c r="D45" s="74" t="s">
+        <v>658</v>
       </c>
       <c r="E45" s="50"/>
       <c r="F45" s="5" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -7605,30 +7639,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="F1" s="71" t="s">
+        <v>663</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>26</v>
@@ -7639,13 +7673,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>30</v>
@@ -7656,13 +7690,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>34</v>
@@ -7673,13 +7707,13 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>38</v>
@@ -7690,13 +7724,13 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>42</v>
@@ -7707,13 +7741,13 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>46</v>
@@ -7724,13 +7758,13 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>50</v>
@@ -7741,13 +7775,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>54</v>
@@ -7758,13 +7792,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>58</v>
@@ -7775,13 +7809,13 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>62</v>
@@ -7792,13 +7826,13 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>66</v>
@@ -7809,13 +7843,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>70</v>
@@ -7826,13 +7860,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>74</v>
@@ -7843,13 +7877,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>78</v>
@@ -7860,13 +7894,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>89</v>
@@ -7877,16 +7911,16 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="F17" s="5">
         <v>4.0</v>
@@ -7894,16 +7928,16 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F18" s="5">
         <v>4.0</v>
@@ -7911,16 +7945,16 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F19" s="5">
         <v>4.0</v>
@@ -7928,16 +7962,16 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F20" s="5">
         <v>4.0</v>
@@ -7966,652 +8000,652 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
-        <v>682</v>
-      </c>
-      <c r="E1" s="73" t="s">
+      <c r="D1" s="79" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1" s="77" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="76" t="s">
-        <v>683</v>
+      <c r="A2" s="80" t="s">
+        <v>684</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>684</v>
-      </c>
-      <c r="C2" s="77" t="s">
         <v>685</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>686</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="76" t="s">
-        <v>686</v>
+      <c r="A3" s="80" t="s">
+        <v>687</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>687</v>
-      </c>
-      <c r="C3" s="77" t="s">
         <v>688</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>689</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="76" t="s">
-        <v>689</v>
+      <c r="A4" s="80" t="s">
+        <v>690</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>690</v>
-      </c>
-      <c r="C4" s="77" t="s">
         <v>691</v>
+      </c>
+      <c r="C4" s="81" t="s">
+        <v>692</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
     <row r="5">
-      <c r="A5" s="76" t="s">
-        <v>692</v>
+      <c r="A5" s="80" t="s">
+        <v>693</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>693</v>
-      </c>
-      <c r="C5" s="77" t="s">
         <v>694</v>
+      </c>
+      <c r="C5" s="81" t="s">
+        <v>695</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6">
-      <c r="A6" s="76" t="s">
-        <v>695</v>
+      <c r="A6" s="80" t="s">
+        <v>696</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>696</v>
-      </c>
-      <c r="C6" s="77" t="s">
         <v>697</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
+      <c r="C6" s="81" t="s">
+        <v>698</v>
+      </c>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7">
-      <c r="A7" s="76" t="s">
-        <v>698</v>
+      <c r="A7" s="80" t="s">
+        <v>699</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>699</v>
-      </c>
-      <c r="C7" s="77" t="s">
         <v>700</v>
+      </c>
+      <c r="C7" s="81" t="s">
+        <v>701</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8">
-      <c r="A8" s="76" t="s">
-        <v>701</v>
+      <c r="A8" s="80" t="s">
+        <v>702</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>702</v>
-      </c>
-      <c r="C8" s="77" t="s">
         <v>703</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>704</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="76" t="s">
-        <v>704</v>
+      <c r="A9" s="80" t="s">
+        <v>705</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>705</v>
-      </c>
-      <c r="C9" s="77" t="s">
         <v>706</v>
+      </c>
+      <c r="C9" s="81" t="s">
+        <v>707</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="76" t="s">
-        <v>707</v>
+      <c r="A10" s="80" t="s">
+        <v>708</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>708</v>
-      </c>
-      <c r="C10" s="77" t="s">
         <v>709</v>
+      </c>
+      <c r="C10" s="81" t="s">
+        <v>710</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="76" t="s">
-        <v>710</v>
+      <c r="A11" s="80" t="s">
+        <v>711</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>711</v>
-      </c>
-      <c r="C11" s="77" t="s">
         <v>712</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>713</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="76" t="s">
-        <v>713</v>
+      <c r="A12" s="80" t="s">
+        <v>714</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>714</v>
-      </c>
-      <c r="C12" s="77" t="s">
         <v>715</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>716</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="76" t="s">
-        <v>716</v>
+      <c r="A13" s="80" t="s">
+        <v>717</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>717</v>
-      </c>
-      <c r="C13" s="77" t="s">
         <v>718</v>
+      </c>
+      <c r="C13" s="81" t="s">
+        <v>719</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="76" t="s">
-        <v>719</v>
+      <c r="A14" s="80" t="s">
+        <v>720</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>720</v>
-      </c>
-      <c r="C14" s="77" t="s">
         <v>721</v>
+      </c>
+      <c r="C14" s="81" t="s">
+        <v>722</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="76" t="s">
-        <v>722</v>
+      <c r="A15" s="80" t="s">
+        <v>723</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>723</v>
-      </c>
-      <c r="C15" s="77" t="s">
         <v>724</v>
+      </c>
+      <c r="C15" s="81" t="s">
+        <v>725</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="76" t="s">
-        <v>725</v>
+      <c r="A16" s="80" t="s">
+        <v>726</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>726</v>
-      </c>
-      <c r="C16" s="77" t="s">
         <v>727</v>
+      </c>
+      <c r="C16" s="81" t="s">
+        <v>728</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17">
-      <c r="A17" s="76" t="s">
-        <v>728</v>
+      <c r="A17" s="80" t="s">
+        <v>729</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>729</v>
-      </c>
-      <c r="C17" s="77" t="s">
-        <v>697</v>
+        <v>730</v>
+      </c>
+      <c r="C17" s="81" t="s">
+        <v>698</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="76" t="s">
-        <v>730</v>
+      <c r="A18" s="80" t="s">
+        <v>731</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>731</v>
-      </c>
-      <c r="C18" s="77" t="s">
         <v>732</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>733</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="76" t="s">
-        <v>733</v>
+      <c r="A19" s="80" t="s">
+        <v>734</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>735</v>
-      </c>
-      <c r="D19" s="79" t="s">
         <v>736</v>
       </c>
+      <c r="D19" s="83" t="s">
+        <v>737</v>
+      </c>
       <c r="E19" s="17"/>
     </row>
     <row r="20">
-      <c r="A20" s="76" t="s">
-        <v>737</v>
+      <c r="A20" s="80" t="s">
+        <v>738</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>738</v>
-      </c>
-      <c r="C20" s="80" t="s">
         <v>739</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>740</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="76" t="s">
-        <v>740</v>
+      <c r="A21" s="80" t="s">
+        <v>741</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>741</v>
-      </c>
-      <c r="C21" s="80" t="s">
         <v>742</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>743</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="76" t="s">
-        <v>743</v>
+      <c r="A22" s="80" t="s">
+        <v>744</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>735</v>
-      </c>
-      <c r="D22" s="80" t="s">
-        <v>745</v>
+        <v>736</v>
+      </c>
+      <c r="D22" s="84" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="76" t="s">
-        <v>746</v>
+      <c r="A23" s="80" t="s">
+        <v>747</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>747</v>
-      </c>
-      <c r="C23" s="77" t="s">
         <v>748</v>
+      </c>
+      <c r="C23" s="81" t="s">
+        <v>749</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
     <row r="24">
-      <c r="A24" s="76" t="s">
-        <v>749</v>
+      <c r="A24" s="80" t="s">
+        <v>750</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>750</v>
-      </c>
-      <c r="C24" s="81" t="s">
         <v>751</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>752</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
     <row r="25">
-      <c r="A25" s="82" t="s">
-        <v>752</v>
-      </c>
-      <c r="B25" s="83" t="s">
+      <c r="A25" s="86" t="s">
         <v>753</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="B25" s="87" t="s">
         <v>754</v>
       </c>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
+      <c r="C25" s="88" t="s">
+        <v>755</v>
+      </c>
+      <c r="D25" s="89"/>
+      <c r="E25" s="89"/>
     </row>
     <row r="26">
-      <c r="A26" s="76" t="s">
-        <v>755</v>
+      <c r="A26" s="80" t="s">
+        <v>756</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>756</v>
-      </c>
-      <c r="C26" s="77" t="s">
         <v>757</v>
+      </c>
+      <c r="C26" s="81" t="s">
+        <v>758</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
     <row r="27">
-      <c r="A27" s="76" t="s">
-        <v>758</v>
+      <c r="A27" s="80" t="s">
+        <v>759</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>759</v>
-      </c>
-      <c r="C27" s="77" t="s">
         <v>760</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>761</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
     <row r="28">
-      <c r="A28" s="76" t="s">
-        <v>761</v>
+      <c r="A28" s="80" t="s">
+        <v>762</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>762</v>
-      </c>
-      <c r="C28" s="77" t="s">
         <v>763</v>
+      </c>
+      <c r="C28" s="81" t="s">
+        <v>764</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
     <row r="29">
-      <c r="A29" s="76" t="s">
-        <v>764</v>
+      <c r="A29" s="80" t="s">
+        <v>765</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>765</v>
-      </c>
-      <c r="C29" s="77" t="s">
         <v>766</v>
+      </c>
+      <c r="C29" s="81" t="s">
+        <v>767</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
     </row>
     <row r="30">
-      <c r="A30" s="76" t="s">
-        <v>767</v>
+      <c r="A30" s="80" t="s">
+        <v>768</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>768</v>
-      </c>
-      <c r="C30" s="77" t="s">
         <v>769</v>
+      </c>
+      <c r="C30" s="81" t="s">
+        <v>770</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31">
-      <c r="A31" s="76" t="s">
-        <v>770</v>
+      <c r="A31" s="80" t="s">
+        <v>771</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>771</v>
-      </c>
-      <c r="C31" s="77" t="s">
         <v>772</v>
+      </c>
+      <c r="C31" s="81" t="s">
+        <v>773</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
     <row r="32">
-      <c r="A32" s="76" t="s">
-        <v>773</v>
+      <c r="A32" s="80" t="s">
+        <v>774</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>774</v>
-      </c>
-      <c r="C32" s="77" t="s">
         <v>775</v>
+      </c>
+      <c r="C32" s="81" t="s">
+        <v>776</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
     <row r="33">
-      <c r="A33" s="76" t="s">
-        <v>776</v>
+      <c r="A33" s="80" t="s">
+        <v>777</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>777</v>
-      </c>
-      <c r="C33" s="77" t="s">
         <v>778</v>
+      </c>
+      <c r="C33" s="81" t="s">
+        <v>779</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
     <row r="34">
-      <c r="A34" s="76" t="s">
-        <v>779</v>
+      <c r="A34" s="80" t="s">
+        <v>780</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>780</v>
-      </c>
-      <c r="C34" s="77" t="s">
         <v>781</v>
+      </c>
+      <c r="C34" s="81" t="s">
+        <v>782</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
     <row r="35">
-      <c r="A35" s="76" t="s">
-        <v>782</v>
+      <c r="A35" s="80" t="s">
+        <v>783</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>783</v>
-      </c>
-      <c r="C35" s="77" t="s">
         <v>784</v>
+      </c>
+      <c r="C35" s="81" t="s">
+        <v>785</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
     <row r="36">
-      <c r="A36" s="76" t="s">
-        <v>785</v>
+      <c r="A36" s="80" t="s">
+        <v>786</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>786</v>
-      </c>
-      <c r="C36" s="86" t="s">
         <v>787</v>
+      </c>
+      <c r="C36" s="90" t="s">
+        <v>788</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
     </row>
     <row r="37">
-      <c r="A37" s="76" t="s">
-        <v>788</v>
+      <c r="A37" s="80" t="s">
+        <v>789</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>789</v>
-      </c>
-      <c r="C37" s="86" t="s">
         <v>790</v>
+      </c>
+      <c r="C37" s="90" t="s">
+        <v>791</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
     </row>
     <row r="38">
-      <c r="A38" s="76" t="s">
-        <v>791</v>
+      <c r="A38" s="80" t="s">
+        <v>792</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>792</v>
-      </c>
-      <c r="C38" s="86" t="s">
         <v>793</v>
+      </c>
+      <c r="C38" s="90" t="s">
+        <v>794</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
     </row>
     <row r="39">
-      <c r="A39" s="76" t="s">
-        <v>794</v>
+      <c r="A39" s="80" t="s">
+        <v>795</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>687</v>
-      </c>
-      <c r="C39" s="80" t="s">
-        <v>795</v>
+        <v>688</v>
+      </c>
+      <c r="C39" s="84" t="s">
+        <v>796</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
     </row>
     <row r="40">
-      <c r="A40" s="76" t="s">
-        <v>796</v>
+      <c r="A40" s="80" t="s">
+        <v>797</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>797</v>
-      </c>
-      <c r="C40" s="80" t="s">
         <v>798</v>
+      </c>
+      <c r="C40" s="84" t="s">
+        <v>799</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
     </row>
     <row r="41">
-      <c r="A41" s="76" t="s">
-        <v>799</v>
+      <c r="A41" s="80" t="s">
+        <v>800</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>800</v>
-      </c>
-      <c r="C41" s="87" t="s">
         <v>801</v>
+      </c>
+      <c r="C41" s="91" t="s">
+        <v>802</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
     </row>
     <row r="42">
-      <c r="A42" s="76" t="s">
-        <v>802</v>
+      <c r="A42" s="80" t="s">
+        <v>803</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>803</v>
-      </c>
-      <c r="C42" s="88" t="s">
         <v>804</v>
       </c>
-      <c r="D42" s="89"/>
-      <c r="E42" s="89"/>
+      <c r="C42" s="92" t="s">
+        <v>805</v>
+      </c>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
     </row>
     <row r="43">
-      <c r="A43" s="76" t="s">
-        <v>805</v>
+      <c r="A43" s="80" t="s">
+        <v>806</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>806</v>
-      </c>
-      <c r="C43" s="90" t="s">
         <v>807</v>
       </c>
+      <c r="C43" s="94" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="76" t="s">
-        <v>808</v>
+      <c r="A44" s="80" t="s">
+        <v>809</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>809</v>
-      </c>
-      <c r="C44" s="90" t="s">
         <v>810</v>
       </c>
+      <c r="C44" s="94" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="76" t="s">
-        <v>811</v>
+      <c r="A45" s="80" t="s">
+        <v>812</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>812</v>
-      </c>
-      <c r="C45" s="91" t="s">
         <v>813</v>
       </c>
+      <c r="C45" s="95" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="76" t="s">
-        <v>814</v>
+      <c r="A46" s="80" t="s">
+        <v>815</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>815</v>
-      </c>
-      <c r="C46" s="88" t="s">
         <v>816</v>
       </c>
-      <c r="D46" s="92"/>
-      <c r="E46" s="92"/>
+      <c r="C46" s="92" t="s">
+        <v>817</v>
+      </c>
+      <c r="D46" s="96"/>
+      <c r="E46" s="96"/>
     </row>
     <row r="47">
-      <c r="A47" s="76" t="s">
-        <v>817</v>
+      <c r="A47" s="80" t="s">
+        <v>818</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>818</v>
-      </c>
-      <c r="C47" s="88" t="s">
         <v>819</v>
       </c>
-      <c r="D47" s="92"/>
-      <c r="E47" s="92"/>
+      <c r="C47" s="92" t="s">
+        <v>820</v>
+      </c>
+      <c r="D47" s="96"/>
+      <c r="E47" s="96"/>
     </row>
     <row r="48">
-      <c r="A48" s="76" t="s">
-        <v>820</v>
+      <c r="A48" s="80" t="s">
+        <v>821</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="C48" s="88" t="s">
         <v>822</v>
       </c>
-      <c r="D48" s="92"/>
-      <c r="E48" s="92"/>
+      <c r="C48" s="92" t="s">
+        <v>823</v>
+      </c>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
     </row>
     <row r="49">
-      <c r="A49" s="76" t="s">
-        <v>823</v>
+      <c r="A49" s="80" t="s">
+        <v>824</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>824</v>
-      </c>
-      <c r="C49" s="91" t="s">
         <v>825</v>
       </c>
-      <c r="D49" s="92"/>
-      <c r="E49" s="92"/>
+      <c r="C49" s="95" t="s">
+        <v>826</v>
+      </c>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
     </row>
     <row r="50">
-      <c r="A50" s="76" t="s">
-        <v>826</v>
+      <c r="A50" s="80" t="s">
+        <v>827</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>827</v>
-      </c>
-      <c r="C50" s="91" t="s">
         <v>828</v>
+      </c>
+      <c r="C50" s="95" t="s">
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -8640,10 +8674,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
@@ -8669,12 +8703,12 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -8701,12 +8735,12 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -8759,134 +8793,134 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="97" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E1" s="62" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F1" s="62" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>835</v>
-      </c>
-      <c r="H1" s="94" t="s">
-        <v>488</v>
+        <v>836</v>
+      </c>
+      <c r="H1" s="98" t="s">
+        <v>489</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>838</v>
-      </c>
-      <c r="F2" s="70"/>
+        <v>839</v>
+      </c>
+      <c r="F2" s="74"/>
       <c r="H2" s="5" t="s">
-        <v>839</v>
-      </c>
-      <c r="I2" s="95" t="s">
         <v>840</v>
+      </c>
+      <c r="I2" s="99" t="s">
+        <v>841</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>842</v>
-      </c>
-      <c r="F3" s="70"/>
+        <v>843</v>
+      </c>
+      <c r="F3" s="74"/>
       <c r="H3" s="5" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="F4" s="70"/>
+        <v>847</v>
+      </c>
+      <c r="F4" s="74"/>
       <c r="H4" s="5" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="F5" s="74"/>
+      <c r="H5" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>848</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>849</v>
-      </c>
-      <c r="F5" s="70"/>
-      <c r="H5" s="5" t="s">
-        <v>843</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>851</v>
-      </c>
-      <c r="F6" s="70"/>
+        <v>852</v>
+      </c>
+      <c r="F6" s="74"/>
       <c r="H6" s="5" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>853</v>
-      </c>
-      <c r="F7" s="70"/>
+        <v>854</v>
+      </c>
+      <c r="F7" s="74"/>
       <c r="H7" s="5" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
   </sheetData>
@@ -8906,16 +8940,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -8930,13 +8964,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -8974,13 +9008,13 @@
     </row>
     <row r="5">
       <c r="A5" s="11" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -8996,10 +9030,10 @@
         <v>0</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -9013,10 +9047,10 @@
     <row r="7">
       <c r="A7" s="11"/>
       <c r="B7" s="11" t="s">
+        <v>867</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>866</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>865</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -9030,10 +9064,10 @@
     <row r="8">
       <c r="A8" s="11"/>
       <c r="B8" s="11" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -9047,10 +9081,10 @@
     <row r="9">
       <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -9076,10 +9110,10 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -9093,10 +9127,10 @@
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>871</v>
-      </c>
-      <c r="B12" s="96" t="s">
         <v>872</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>873</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -9110,10 +9144,10 @@
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>873</v>
-      </c>
-      <c r="B13" s="96" t="s">
         <v>874</v>
+      </c>
+      <c r="B13" s="100" t="s">
+        <v>875</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -9140,10 +9174,10 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>875</v>
-      </c>
-      <c r="B15" s="95" t="s">
         <v>876</v>
+      </c>
+      <c r="B15" s="99" t="s">
+        <v>877</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -9157,27 +9191,27 @@
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
-        <v>877</v>
-      </c>
-      <c r="B16" s="94" t="s">
+        <v>878</v>
+      </c>
+      <c r="B16" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
-        <v>878</v>
-      </c>
-      <c r="B17" s="94" t="s">
         <v>879</v>
+      </c>
+      <c r="B17" s="98" t="s">
+        <v>880</v>
       </c>
     </row>
     <row r="18">
@@ -9199,46 +9233,46 @@
       <c r="A23" s="11"/>
     </row>
     <row r="24">
-      <c r="A24" s="97" t="s">
-        <v>880</v>
-      </c>
-      <c r="B24" s="98" t="s">
+      <c r="A24" s="101" t="s">
         <v>881</v>
       </c>
+      <c r="B24" s="102" t="s">
+        <v>882</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="97" t="s">
-        <v>882</v>
-      </c>
-      <c r="B25" s="98" t="s">
+      <c r="A25" s="101" t="s">
         <v>883</v>
       </c>
+      <c r="B25" s="102" t="s">
+        <v>884</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="97" t="s">
-        <v>884</v>
-      </c>
-      <c r="B26" s="99" t="s">
+      <c r="A26" s="101" t="s">
         <v>885</v>
       </c>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
+      <c r="B26" s="103" t="s">
+        <v>886</v>
+      </c>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="104"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="104"/>
     </row>
     <row r="27" hidden="1">
       <c r="A27" s="11" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="28" hidden="1">
       <c r="A28" s="11" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
     <row r="29">
@@ -9276,66 +9310,66 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>890</v>
-      </c>
-      <c r="C2" s="102" t="s">
         <v>891</v>
+      </c>
+      <c r="C2" s="106" t="s">
+        <v>892</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>892</v>
-      </c>
-      <c r="C3" s="102" t="s">
         <v>893</v>
+      </c>
+      <c r="C3" s="106" t="s">
+        <v>894</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>894</v>
-      </c>
-      <c r="C4" s="102" t="s">
         <v>895</v>
+      </c>
+      <c r="C4" s="106" t="s">
+        <v>896</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>896</v>
-      </c>
-      <c r="C5" s="102" t="s">
         <v>897</v>
+      </c>
+      <c r="C5" s="106" t="s">
+        <v>898</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>843</v>
-      </c>
-      <c r="C6" s="103" t="s">
-        <v>898</v>
-      </c>
-      <c r="D6" s="104"/>
+        <v>844</v>
+      </c>
+      <c r="C6" s="107" t="s">
+        <v>899</v>
+      </c>
+      <c r="D6" s="108"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>899</v>
-      </c>
-      <c r="C7" s="103" t="s">
         <v>900</v>
+      </c>
+      <c r="C7" s="107" t="s">
+        <v>901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes and id updates
aacar use ascending aorta instead of aorta
aacar-6 fix missing left atrium branches

bolew external carotid nerve plexus instead of just nerve, replace
FMA ids with ILX and UBERON

bromo replace FMA ids with ILX
</commit_message>
<xml_diff>
--- a/models/bronchomotor/source/bronchomotor.xlsx
+++ b/models/bronchomotor/source/bronchomotor.xlsx
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="942">
   <si>
     <t>id</t>
   </si>
@@ -2492,7 +2492,7 @@
     <t>Wall of larynx</t>
   </si>
   <si>
-    <t>FMA:64182</t>
+    <t>ILX:0738326</t>
   </si>
   <si>
     <t>BM_43</t>
@@ -2501,7 +2501,7 @@
     <t>Wall of trachea</t>
   </si>
   <si>
-    <t>FMA:7470</t>
+    <t>ILX:0793684</t>
   </si>
   <si>
     <t>BM_44</t>
@@ -2510,7 +2510,7 @@
     <t>Wall of bronchus</t>
   </si>
   <si>
-    <t>FMA:67480</t>
+    <t>ILX:0793764</t>
   </si>
   <si>
     <t>BM_45</t>
@@ -2519,7 +2519,7 @@
     <t>Wall of bronchiole</t>
   </si>
   <si>
-    <t>FMA:74655</t>
+    <t>ILX:0793765</t>
   </si>
   <si>
     <t>BM_46</t>
@@ -2528,7 +2528,7 @@
     <t>Wall of terminal bronchiole</t>
   </si>
   <si>
-    <t>FMA:62792</t>
+    <t>ILX:0775392</t>
   </si>
   <si>
     <t>BM_47</t>
@@ -2796,6 +2796,9 @@
   </si>
   <si>
     <t>Bernard de Bono</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-4577-8954</t>
   </si>
   <si>
     <t>Don Bolser</t>
@@ -3002,11 +3005,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color rgb="FF555555"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -3039,6 +3037,10 @@
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <b/>
@@ -3127,7 +3129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3400,13 +3402,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -3422,30 +3424,33 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
@@ -3796,8 +3801,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" s="112" t="s">
+        <v>910</v>
+      </c>
       <c r="B5" s="111" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="C5" s="111" t="s">
         <v>905</v>
@@ -3808,8 +3816,9 @@
     <hyperlink r:id="rId1" ref="A2"/>
     <hyperlink r:id="rId2" ref="A3"/>
     <hyperlink r:id="rId3" ref="A4"/>
+    <hyperlink r:id="rId4" ref="A5"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -3827,123 +3836,123 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="112" t="s">
-        <v>911</v>
-      </c>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="113" t="s">
         <v>912</v>
+      </c>
+      <c r="B1" s="113" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>913</v>
-      </c>
-      <c r="B2" s="113" t="s">
         <v>914</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>915</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31" t="s">
-        <v>915</v>
-      </c>
-      <c r="B3" s="113" t="s">
         <v>916</v>
+      </c>
+      <c r="B3" s="114" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>917</v>
-      </c>
-      <c r="B4" s="113" t="s">
         <v>918</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>919</v>
-      </c>
-      <c r="B5" s="113" t="s">
         <v>920</v>
+      </c>
+      <c r="B5" s="114" t="s">
+        <v>921</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>921</v>
-      </c>
-      <c r="B6" s="113" t="s">
         <v>922</v>
+      </c>
+      <c r="B6" s="114" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>923</v>
-      </c>
-      <c r="B7" s="113" t="s">
         <v>924</v>
+      </c>
+      <c r="B7" s="114" t="s">
+        <v>925</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>925</v>
-      </c>
-      <c r="B8" s="113" t="s">
         <v>926</v>
+      </c>
+      <c r="B8" s="114" t="s">
+        <v>927</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>927</v>
-      </c>
-      <c r="B9" s="113" t="s">
         <v>928</v>
+      </c>
+      <c r="B9" s="114" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>929</v>
-      </c>
-      <c r="B10" s="113" t="s">
         <v>930</v>
+      </c>
+      <c r="B10" s="114" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="31" t="s">
-        <v>931</v>
-      </c>
-      <c r="B11" s="113" t="s">
         <v>932</v>
+      </c>
+      <c r="B11" s="114" t="s">
+        <v>933</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="31" t="s">
-        <v>933</v>
-      </c>
-      <c r="B12" s="113" t="s">
         <v>934</v>
+      </c>
+      <c r="B12" s="114" t="s">
+        <v>935</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="31" t="s">
-        <v>935</v>
-      </c>
-      <c r="B13" s="113" t="s">
         <v>936</v>
+      </c>
+      <c r="B13" s="114" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="31" t="s">
-        <v>937</v>
-      </c>
-      <c r="B14" s="113" t="s">
         <v>938</v>
+      </c>
+      <c r="B14" s="114" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="31" t="s">
-        <v>939</v>
-      </c>
-      <c r="B15" s="113" t="s">
         <v>940</v>
+      </c>
+      <c r="B15" s="114" t="s">
+        <v>941</v>
       </c>
     </row>
   </sheetData>
@@ -6404,7 +6413,7 @@
     <col customWidth="1" min="8" max="8" width="5.75"/>
     <col customWidth="1" min="9" max="9" width="6.5"/>
     <col customWidth="1" min="10" max="10" width="6.13"/>
-    <col customWidth="1" min="12" max="12" width="27.38"/>
+    <col customWidth="1" min="12" max="12" width="33.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8559,7 +8568,7 @@
       <c r="B43" s="11" t="s">
         <v>807</v>
       </c>
-      <c r="C43" s="94" t="s">
+      <c r="C43" s="5" t="s">
         <v>808</v>
       </c>
     </row>
@@ -8570,7 +8579,7 @@
       <c r="B44" s="11" t="s">
         <v>810</v>
       </c>
-      <c r="C44" s="94" t="s">
+      <c r="C44" s="5" t="s">
         <v>811</v>
       </c>
     </row>
@@ -8581,7 +8590,7 @@
       <c r="B45" s="4" t="s">
         <v>813</v>
       </c>
-      <c r="C45" s="95" t="s">
+      <c r="C45" s="5" t="s">
         <v>814</v>
       </c>
     </row>
@@ -8592,11 +8601,10 @@
       <c r="B46" s="5" t="s">
         <v>816</v>
       </c>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
+      <c r="E46" s="94"/>
     </row>
     <row r="47">
       <c r="A47" s="80" t="s">
@@ -8605,11 +8613,10 @@
       <c r="B47" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="C47" s="92" t="s">
+      <c r="C47" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="96"/>
+      <c r="E47" s="94"/>
     </row>
     <row r="48">
       <c r="A48" s="80" t="s">
@@ -8618,11 +8625,11 @@
       <c r="B48" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="C48" s="92" t="s">
+      <c r="C48" s="95" t="s">
         <v>823</v>
       </c>
-      <c r="D48" s="96"/>
-      <c r="E48" s="96"/>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
     </row>
     <row r="49">
       <c r="A49" s="80" t="s">
@@ -8631,11 +8638,11 @@
       <c r="B49" s="4" t="s">
         <v>825</v>
       </c>
-      <c r="C49" s="95" t="s">
+      <c r="C49" s="96" t="s">
         <v>826</v>
       </c>
-      <c r="D49" s="96"/>
-      <c r="E49" s="96"/>
+      <c r="D49" s="94"/>
+      <c r="E49" s="94"/>
     </row>
     <row r="50">
       <c r="A50" s="80" t="s">
@@ -8644,7 +8651,7 @@
       <c r="B50" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="C50" s="95" t="s">
+      <c r="C50" s="96" t="s">
         <v>829</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bromo fix T2 gray ramus id
</commit_message>
<xml_diff>
--- a/models/bronchomotor/source/bronchomotor.xlsx
+++ b/models/bronchomotor/source/bronchomotor.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -971,7 +971,7 @@
     <t>B86</t>
   </si>
   <si>
-    <t>ILX:0791105</t>
+    <t>ILX:0739303</t>
   </si>
   <si>
     <t>T2 gray ramus</t>
@@ -2588,7 +2588,7 @@
     <t>ilxtr:neuron-type-bromo-1</t>
   </si>
   <si>
-    <t>PMID: 8300416, PMID: 3198482, PMID: 2384334</t>
+    <t>PMID:8300416, PMID:3198482, PMID:2384334</t>
   </si>
   <si>
     <t>sympathetic pre-ganglionic neuron</t>
@@ -2759,10 +2759,10 @@
     <t>https://pubmed.ncbi.nlm.nih.gov/3198482</t>
   </si>
   <si>
-    <t xml:space="preserve">PMID:18579364 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/18579364 </t>
+    <t>PMID:18579364</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/18579364</t>
   </si>
   <si>
     <t>https://doi.org/10.1016/B978-0-444-53491-0.09985-5</t>
@@ -2898,7 +2898,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="31">
+  <fonts count="32">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3029,6 +3029,12 @@
     </font>
     <font>
       <u/>
+      <sz val="11.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Inconsolata"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -3129,7 +3135,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3237,6 +3243,9 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
@@ -3437,11 +3446,14 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3450,11 +3462,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -3755,6 +3767,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="20.13"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
@@ -3768,46 +3783,46 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="111" t="s">
         <v>903</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="112" t="s">
         <v>904</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="113" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="111" t="s">
         <v>906</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>907</v>
       </c>
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="113" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="111" t="s">
         <v>908</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>909</v>
       </c>
-      <c r="C4" s="111" t="s">
+      <c r="C4" s="113" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="112" t="s">
+      <c r="A5" s="114" t="s">
         <v>910</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="113" t="s">
         <v>911</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="C5" s="113" t="s">
         <v>905</v>
       </c>
     </row>
@@ -3836,10 +3851,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="115" t="s">
         <v>912</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="115" t="s">
         <v>913</v>
       </c>
     </row>
@@ -3847,7 +3862,7 @@
       <c r="A2" s="31" t="s">
         <v>914</v>
       </c>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="116" t="s">
         <v>915</v>
       </c>
     </row>
@@ -3855,7 +3870,7 @@
       <c r="A3" s="31" t="s">
         <v>916</v>
       </c>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="116" t="s">
         <v>917</v>
       </c>
     </row>
@@ -3863,7 +3878,7 @@
       <c r="A4" s="31" t="s">
         <v>918</v>
       </c>
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="116" t="s">
         <v>919</v>
       </c>
     </row>
@@ -3871,7 +3886,7 @@
       <c r="A5" s="31" t="s">
         <v>920</v>
       </c>
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="116" t="s">
         <v>921</v>
       </c>
     </row>
@@ -3879,7 +3894,7 @@
       <c r="A6" s="31" t="s">
         <v>922</v>
       </c>
-      <c r="B6" s="114" t="s">
+      <c r="B6" s="116" t="s">
         <v>923</v>
       </c>
     </row>
@@ -3887,7 +3902,7 @@
       <c r="A7" s="31" t="s">
         <v>924</v>
       </c>
-      <c r="B7" s="114" t="s">
+      <c r="B7" s="116" t="s">
         <v>925</v>
       </c>
     </row>
@@ -3895,7 +3910,7 @@
       <c r="A8" s="31" t="s">
         <v>926</v>
       </c>
-      <c r="B8" s="114" t="s">
+      <c r="B8" s="116" t="s">
         <v>927</v>
       </c>
     </row>
@@ -3903,7 +3918,7 @@
       <c r="A9" s="31" t="s">
         <v>928</v>
       </c>
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="116" t="s">
         <v>929</v>
       </c>
     </row>
@@ -3911,7 +3926,7 @@
       <c r="A10" s="31" t="s">
         <v>930</v>
       </c>
-      <c r="B10" s="114" t="s">
+      <c r="B10" s="116" t="s">
         <v>931</v>
       </c>
     </row>
@@ -3919,7 +3934,7 @@
       <c r="A11" s="31" t="s">
         <v>932</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="B11" s="116" t="s">
         <v>933</v>
       </c>
     </row>
@@ -3927,7 +3942,7 @@
       <c r="A12" s="31" t="s">
         <v>934</v>
       </c>
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="116" t="s">
         <v>935</v>
       </c>
     </row>
@@ -3935,7 +3950,7 @@
       <c r="A13" s="31" t="s">
         <v>936</v>
       </c>
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="116" t="s">
         <v>937</v>
       </c>
     </row>
@@ -3943,7 +3958,7 @@
       <c r="A14" s="31" t="s">
         <v>938</v>
       </c>
-      <c r="B14" s="114" t="s">
+      <c r="B14" s="116" t="s">
         <v>939</v>
       </c>
     </row>
@@ -3951,7 +3966,7 @@
       <c r="A15" s="31" t="s">
         <v>940</v>
       </c>
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="116" t="s">
         <v>941</v>
       </c>
     </row>
@@ -5241,7 +5256,7 @@
       <c r="A89" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B89" s="37" t="s">
         <v>301</v>
       </c>
       <c r="C89" s="21" t="s">
@@ -5397,7 +5412,7 @@
       <c r="A102" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="B102" s="37" t="s">
+      <c r="B102" s="38" t="s">
         <v>340</v>
       </c>
       <c r="C102" s="5" t="s">
@@ -5411,7 +5426,7 @@
       <c r="A103" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="B103" s="37" t="s">
+      <c r="B103" s="38" t="s">
         <v>344</v>
       </c>
       <c r="C103" s="5" t="s">
@@ -5423,7 +5438,7 @@
       <c r="A104" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="B104" s="37" t="s">
+      <c r="B104" s="38" t="s">
         <v>347</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -5441,7 +5456,7 @@
       <c r="A105" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="B105" s="37" t="s">
+      <c r="B105" s="38" t="s">
         <v>350</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -5449,138 +5464,138 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="38" t="s">
+      <c r="A106" s="39" t="s">
         <v>352</v>
       </c>
-      <c r="B106" s="39" t="s">
+      <c r="B106" s="40" t="s">
         <v>353</v>
       </c>
-      <c r="C106" s="40" t="s">
+      <c r="C106" s="41" t="s">
         <v>354</v>
       </c>
-      <c r="D106" s="41"/>
-      <c r="E106" s="41"/>
-      <c r="F106" s="41"/>
-      <c r="G106" s="41"/>
-      <c r="H106" s="41"/>
-      <c r="I106" s="42" t="s">
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="42"/>
+      <c r="I106" s="43" t="s">
         <v>355</v>
       </c>
-      <c r="J106" s="41"/>
-      <c r="K106" s="41"/>
-      <c r="L106" s="41"/>
-      <c r="M106" s="40" t="s">
+      <c r="J106" s="42"/>
+      <c r="K106" s="42"/>
+      <c r="L106" s="42"/>
+      <c r="M106" s="41" t="s">
         <v>356</v>
       </c>
-      <c r="N106" s="40" t="s">
+      <c r="N106" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="O106" s="41"/>
-      <c r="P106" s="41"/>
-      <c r="Q106" s="41"/>
-      <c r="R106" s="41"/>
+      <c r="O106" s="42"/>
+      <c r="P106" s="42"/>
+      <c r="Q106" s="42"/>
+      <c r="R106" s="42"/>
     </row>
     <row r="107">
-      <c r="A107" s="43" t="s">
+      <c r="A107" s="44" t="s">
         <v>358</v>
       </c>
-      <c r="B107" s="39" t="s">
+      <c r="B107" s="40" t="s">
         <v>359</v>
       </c>
-      <c r="C107" s="40" t="s">
+      <c r="C107" s="41" t="s">
         <v>360</v>
       </c>
-      <c r="D107" s="41"/>
-      <c r="E107" s="41"/>
-      <c r="F107" s="41"/>
-      <c r="G107" s="41"/>
-      <c r="H107" s="41"/>
-      <c r="I107" s="42" t="s">
+      <c r="D107" s="42"/>
+      <c r="E107" s="42"/>
+      <c r="F107" s="42"/>
+      <c r="G107" s="42"/>
+      <c r="H107" s="42"/>
+      <c r="I107" s="43" t="s">
         <v>361</v>
       </c>
-      <c r="J107" s="41"/>
-      <c r="K107" s="41"/>
-      <c r="L107" s="41"/>
-      <c r="M107" s="40" t="s">
+      <c r="J107" s="42"/>
+      <c r="K107" s="42"/>
+      <c r="L107" s="42"/>
+      <c r="M107" s="41" t="s">
         <v>362</v>
       </c>
-      <c r="N107" s="40" t="s">
+      <c r="N107" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="O107" s="41"/>
-      <c r="P107" s="41"/>
-      <c r="Q107" s="41"/>
-      <c r="R107" s="41"/>
+      <c r="O107" s="42"/>
+      <c r="P107" s="42"/>
+      <c r="Q107" s="42"/>
+      <c r="R107" s="42"/>
     </row>
     <row r="108">
-      <c r="A108" s="43" t="s">
+      <c r="A108" s="44" t="s">
         <v>363</v>
       </c>
-      <c r="B108" s="44" t="s">
+      <c r="B108" s="45" t="s">
         <v>364</v>
       </c>
-      <c r="C108" s="40" t="s">
+      <c r="C108" s="41" t="s">
         <v>365</v>
       </c>
-      <c r="D108" s="41"/>
-      <c r="E108" s="41"/>
-      <c r="F108" s="41"/>
-      <c r="G108" s="41"/>
-      <c r="H108" s="41"/>
-      <c r="I108" s="42" t="s">
+      <c r="D108" s="42"/>
+      <c r="E108" s="42"/>
+      <c r="F108" s="42"/>
+      <c r="G108" s="42"/>
+      <c r="H108" s="42"/>
+      <c r="I108" s="43" t="s">
         <v>366</v>
       </c>
-      <c r="J108" s="41"/>
-      <c r="K108" s="41"/>
-      <c r="L108" s="41"/>
-      <c r="M108" s="40" t="s">
+      <c r="J108" s="42"/>
+      <c r="K108" s="42"/>
+      <c r="L108" s="42"/>
+      <c r="M108" s="41" t="s">
         <v>367</v>
       </c>
-      <c r="N108" s="40" t="s">
+      <c r="N108" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="O108" s="41"/>
-      <c r="P108" s="41"/>
-      <c r="Q108" s="41"/>
-      <c r="R108" s="41"/>
+      <c r="O108" s="42"/>
+      <c r="P108" s="42"/>
+      <c r="Q108" s="42"/>
+      <c r="R108" s="42"/>
     </row>
     <row r="109">
-      <c r="A109" s="38" t="s">
+      <c r="A109" s="39" t="s">
         <v>368</v>
       </c>
-      <c r="B109" s="44" t="s">
+      <c r="B109" s="45" t="s">
         <v>369</v>
       </c>
-      <c r="C109" s="40" t="s">
+      <c r="C109" s="41" t="s">
         <v>370</v>
       </c>
-      <c r="D109" s="41"/>
-      <c r="E109" s="41"/>
-      <c r="F109" s="41"/>
-      <c r="G109" s="41"/>
-      <c r="H109" s="41"/>
-      <c r="I109" s="42" t="s">
+      <c r="D109" s="42"/>
+      <c r="E109" s="42"/>
+      <c r="F109" s="42"/>
+      <c r="G109" s="42"/>
+      <c r="H109" s="42"/>
+      <c r="I109" s="43" t="s">
         <v>371</v>
       </c>
-      <c r="J109" s="41"/>
-      <c r="K109" s="41"/>
-      <c r="L109" s="41"/>
-      <c r="M109" s="40" t="s">
+      <c r="J109" s="42"/>
+      <c r="K109" s="42"/>
+      <c r="L109" s="42"/>
+      <c r="M109" s="41" t="s">
         <v>372</v>
       </c>
-      <c r="N109" s="40" t="s">
+      <c r="N109" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="O109" s="41"/>
-      <c r="P109" s="41"/>
-      <c r="Q109" s="41"/>
-      <c r="R109" s="41"/>
+      <c r="O109" s="42"/>
+      <c r="P109" s="42"/>
+      <c r="Q109" s="42"/>
+      <c r="R109" s="42"/>
     </row>
     <row r="110">
       <c r="A110" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="B110" s="45" t="s">
+      <c r="B110" s="46" t="s">
         <v>374</v>
       </c>
       <c r="C110" s="5" t="s">
@@ -5592,7 +5607,7 @@
       <c r="A111" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="B111" s="37" t="s">
+      <c r="B111" s="38" t="s">
         <v>377</v>
       </c>
       <c r="C111" s="5" t="s">
@@ -5604,7 +5619,7 @@
       <c r="A112" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="B112" s="37" t="s">
+      <c r="B112" s="38" t="s">
         <v>380</v>
       </c>
       <c r="C112" s="5" t="s">
@@ -5616,7 +5631,7 @@
       <c r="A113" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="B113" s="37" t="s">
+      <c r="B113" s="38" t="s">
         <v>383</v>
       </c>
       <c r="C113" s="5" t="s">
@@ -5628,7 +5643,7 @@
       <c r="A114" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="B114" s="37" t="s">
+      <c r="B114" s="38" t="s">
         <v>386</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -5645,7 +5660,7 @@
       <c r="A115" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="B115" s="37" t="s">
+      <c r="B115" s="38" t="s">
         <v>390</v>
       </c>
       <c r="C115" s="5" t="s">
@@ -5663,14 +5678,14 @@
       <c r="A116" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="B116" s="46" t="s">
+      <c r="B116" s="47" t="s">
         <v>393</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>394</v>
       </c>
       <c r="I116" s="24"/>
-      <c r="M116" s="47" t="s">
+      <c r="M116" s="48" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5678,14 +5693,14 @@
       <c r="A117" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="B117" s="46" t="s">
+      <c r="B117" s="47" t="s">
         <v>397</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>398</v>
       </c>
       <c r="I117" s="24"/>
-      <c r="M117" s="47" t="s">
+      <c r="M117" s="48" t="s">
         <v>399</v>
       </c>
     </row>
@@ -5693,14 +5708,14 @@
       <c r="A118" s="15" t="s">
         <v>400</v>
       </c>
-      <c r="B118" s="46" t="s">
+      <c r="B118" s="47" t="s">
         <v>401</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>402</v>
       </c>
       <c r="I118" s="24"/>
-      <c r="M118" s="47" t="s">
+      <c r="M118" s="48" t="s">
         <v>403</v>
       </c>
     </row>
@@ -5708,14 +5723,14 @@
       <c r="A119" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="B119" s="46" t="s">
+      <c r="B119" s="47" t="s">
         <v>405</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>406</v>
       </c>
       <c r="I119" s="24"/>
-      <c r="M119" s="47" t="s">
+      <c r="M119" s="48" t="s">
         <v>407</v>
       </c>
     </row>
@@ -5735,10 +5750,10 @@
       <c r="A121" s="15" t="s">
         <v>410</v>
       </c>
-      <c r="B121" s="37" t="s">
+      <c r="B121" s="38" t="s">
         <v>411</v>
       </c>
-      <c r="C121" s="48" t="s">
+      <c r="C121" s="49" t="s">
         <v>412</v>
       </c>
       <c r="I121" s="24"/>
@@ -5747,7 +5762,7 @@
       <c r="A122" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B122" s="37" t="s">
+      <c r="B122" s="38" t="s">
         <v>414</v>
       </c>
       <c r="C122" s="5" t="s">
@@ -5759,7 +5774,7 @@
       <c r="A123" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="B123" s="37" t="s">
+      <c r="B123" s="38" t="s">
         <v>417</v>
       </c>
       <c r="C123" s="5" t="s">
@@ -5771,7 +5786,7 @@
       <c r="A124" s="15" t="s">
         <v>419</v>
       </c>
-      <c r="B124" s="37" t="s">
+      <c r="B124" s="38" t="s">
         <v>420</v>
       </c>
       <c r="C124" s="5" t="s">
@@ -5783,7 +5798,7 @@
       <c r="A125" s="12" t="s">
         <v>422</v>
       </c>
-      <c r="B125" s="37" t="s">
+      <c r="B125" s="38" t="s">
         <v>423</v>
       </c>
       <c r="C125" s="5" t="s">
@@ -5795,7 +5810,7 @@
       <c r="A126" s="15" t="s">
         <v>425</v>
       </c>
-      <c r="B126" s="37" t="s">
+      <c r="B126" s="38" t="s">
         <v>426</v>
       </c>
       <c r="C126" s="5" t="s">
@@ -5807,7 +5822,7 @@
       <c r="A127" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="B127" s="37" t="s">
+      <c r="B127" s="38" t="s">
         <v>429</v>
       </c>
       <c r="C127" s="5" t="s">
@@ -5819,7 +5834,7 @@
       <c r="A128" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="B128" s="37" t="s">
+      <c r="B128" s="38" t="s">
         <v>432</v>
       </c>
       <c r="C128" s="5" t="s">
@@ -5831,16 +5846,16 @@
       <c r="A129" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="B129" s="37" t="s">
+      <c r="B129" s="38" t="s">
         <v>411</v>
       </c>
-      <c r="C129" s="48" t="s">
+      <c r="C129" s="49" t="s">
         <v>412</v>
       </c>
       <c r="I129" s="11"/>
     </row>
     <row r="130">
-      <c r="A130" s="49" t="s">
+      <c r="A130" s="50" t="s">
         <v>435</v>
       </c>
       <c r="B130" s="16" t="s">
@@ -5857,7 +5872,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="50" t="s">
+      <c r="A131" s="51" t="s">
         <v>439</v>
       </c>
       <c r="B131" s="16" t="s">
@@ -5875,17 +5890,17 @@
       <c r="I131" s="11"/>
     </row>
     <row r="132">
-      <c r="A132" s="51" t="s">
+      <c r="A132" s="52" t="s">
         <v>442</v>
       </c>
-      <c r="B132" s="52" t="s">
+      <c r="B132" s="53" t="s">
         <v>443</v>
       </c>
-      <c r="C132" s="53" t="s">
+      <c r="C132" s="54" t="s">
         <v>444</v>
       </c>
       <c r="D132" s="11"/>
-      <c r="E132" s="54" t="b">
+      <c r="E132" s="55" t="b">
         <v>1</v>
       </c>
       <c r="F132" s="26" t="s">
@@ -5894,28 +5909,28 @@
       <c r="G132" s="11"/>
       <c r="H132" s="11"/>
       <c r="I132" s="11"/>
-      <c r="J132" s="53"/>
+      <c r="J132" s="54"/>
       <c r="K132" s="11"/>
       <c r="L132" s="11"/>
       <c r="M132" s="11"/>
-      <c r="N132" s="55"/>
+      <c r="N132" s="56"/>
       <c r="O132" s="11"/>
       <c r="P132" s="11"/>
       <c r="Q132" s="11"/>
-      <c r="R132" s="53"/>
+      <c r="R132" s="54"/>
     </row>
     <row r="133">
-      <c r="A133" s="51" t="s">
+      <c r="A133" s="52" t="s">
         <v>446</v>
       </c>
-      <c r="B133" s="52" t="s">
+      <c r="B133" s="53" t="s">
         <v>443</v>
       </c>
-      <c r="C133" s="53" t="s">
+      <c r="C133" s="54" t="s">
         <v>447</v>
       </c>
       <c r="D133" s="11"/>
-      <c r="E133" s="54" t="b">
+      <c r="E133" s="55" t="b">
         <v>1</v>
       </c>
       <c r="F133" s="26" t="s">
@@ -5924,28 +5939,28 @@
       <c r="G133" s="11"/>
       <c r="H133" s="11"/>
       <c r="I133" s="11"/>
-      <c r="J133" s="53"/>
+      <c r="J133" s="54"/>
       <c r="K133" s="11"/>
       <c r="L133" s="11"/>
       <c r="M133" s="11"/>
-      <c r="N133" s="55"/>
+      <c r="N133" s="56"/>
       <c r="O133" s="11"/>
       <c r="P133" s="11"/>
       <c r="Q133" s="11"/>
-      <c r="R133" s="53"/>
+      <c r="R133" s="54"/>
     </row>
     <row r="134">
-      <c r="A134" s="51" t="s">
+      <c r="A134" s="52" t="s">
         <v>449</v>
       </c>
-      <c r="B134" s="52" t="s">
+      <c r="B134" s="53" t="s">
         <v>450</v>
       </c>
-      <c r="C134" s="53" t="s">
+      <c r="C134" s="54" t="s">
         <v>451</v>
       </c>
       <c r="D134" s="11"/>
-      <c r="E134" s="54" t="b">
+      <c r="E134" s="55" t="b">
         <v>1</v>
       </c>
       <c r="F134" s="26" t="s">
@@ -5954,28 +5969,28 @@
       <c r="G134" s="11"/>
       <c r="H134" s="11"/>
       <c r="I134" s="11"/>
-      <c r="J134" s="53"/>
+      <c r="J134" s="54"/>
       <c r="K134" s="11"/>
       <c r="L134" s="11"/>
       <c r="M134" s="11"/>
-      <c r="N134" s="55"/>
+      <c r="N134" s="56"/>
       <c r="O134" s="11"/>
       <c r="P134" s="11"/>
       <c r="Q134" s="11"/>
-      <c r="R134" s="53"/>
+      <c r="R134" s="54"/>
     </row>
     <row r="135">
-      <c r="A135" s="51" t="s">
+      <c r="A135" s="52" t="s">
         <v>452</v>
       </c>
-      <c r="B135" s="52" t="s">
+      <c r="B135" s="53" t="s">
         <v>450</v>
       </c>
-      <c r="C135" s="53" t="s">
+      <c r="C135" s="54" t="s">
         <v>453</v>
       </c>
       <c r="D135" s="11"/>
-      <c r="E135" s="54" t="b">
+      <c r="E135" s="55" t="b">
         <v>1</v>
       </c>
       <c r="F135" s="26" t="s">
@@ -5984,15 +5999,15 @@
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
       <c r="I135" s="11"/>
-      <c r="J135" s="53"/>
+      <c r="J135" s="54"/>
       <c r="K135" s="11"/>
       <c r="L135" s="11"/>
       <c r="M135" s="11"/>
-      <c r="N135" s="55"/>
+      <c r="N135" s="56"/>
       <c r="O135" s="11"/>
       <c r="P135" s="11"/>
       <c r="Q135" s="11"/>
-      <c r="R135" s="53"/>
+      <c r="R135" s="54"/>
     </row>
     <row r="136">
       <c r="A136" s="5" t="s">
@@ -6355,30 +6370,30 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="56">
+      <c r="A155" s="57">
         <v>229.0</v>
       </c>
-      <c r="B155" s="52" t="s">
+      <c r="B155" s="53" t="s">
         <v>436</v>
       </c>
-      <c r="C155" s="53" t="s">
+      <c r="C155" s="54" t="s">
         <v>437</v>
       </c>
       <c r="D155" s="11"/>
-      <c r="E155" s="57" t="b">
+      <c r="E155" s="58" t="b">
         <v>1</v>
       </c>
-      <c r="F155" s="53"/>
+      <c r="F155" s="54"/>
       <c r="G155" s="11"/>
       <c r="H155" s="11"/>
-      <c r="I155" s="58" t="s">
+      <c r="I155" s="59" t="s">
         <v>480</v>
       </c>
-      <c r="J155" s="53"/>
-      <c r="K155" s="58"/>
+      <c r="J155" s="54"/>
+      <c r="K155" s="59"/>
       <c r="L155" s="11"/>
       <c r="M155" s="11"/>
-      <c r="N155" s="55"/>
+      <c r="N155" s="56"/>
       <c r="O155" s="11"/>
       <c r="P155" s="11"/>
       <c r="Q155" s="11"/>
@@ -6420,10 +6435,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -6444,13 +6459,13 @@
       <c r="I1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="62" t="s">
         <v>486</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="L1" s="63" t="s">
         <v>488</v>
       </c>
       <c r="M1" s="4" t="s">
@@ -6461,20 +6476,20 @@
       <c r="A2" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>491</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="51" t="s">
+      <c r="D2" s="65"/>
+      <c r="E2" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="K2" s="65">
+      <c r="K2" s="66">
         <v>6.0</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -6485,14 +6500,14 @@
       <c r="A3" s="5" t="s">
         <v>494</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>495</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="64" t="s">
         <v>496</v>
       </c>
       <c r="D3" s="11"/>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -6501,10 +6516,10 @@
       <c r="G3" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K3" s="65" t="s">
+      <c r="K3" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L3" s="65" t="s">
+      <c r="L3" s="66" t="s">
         <v>500</v>
       </c>
     </row>
@@ -6512,22 +6527,22 @@
       <c r="A4" s="5" t="s">
         <v>501</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>502</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>503</v>
       </c>
-      <c r="K4" s="65">
+      <c r="K4" s="66">
         <v>6.0</v>
       </c>
-      <c r="L4" s="65" t="s">
+      <c r="L4" s="66" t="s">
         <v>27</v>
       </c>
     </row>
@@ -6535,13 +6550,13 @@
       <c r="A5" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>505</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -6550,10 +6565,10 @@
       <c r="G5" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K5" s="65" t="s">
+      <c r="K5" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L5" s="65" t="s">
+      <c r="L5" s="66" t="s">
         <v>507</v>
       </c>
     </row>
@@ -6561,22 +6576,22 @@
       <c r="A6" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="38" t="s">
         <v>509</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="66">
         <v>6.0</v>
       </c>
-      <c r="L6" s="65" t="s">
+      <c r="L6" s="66" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6584,13 +6599,13 @@
       <c r="A7" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="38" t="s">
         <v>512</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -6599,10 +6614,10 @@
       <c r="G7" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K7" s="65" t="s">
+      <c r="K7" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L7" s="65" t="s">
+      <c r="L7" s="66" t="s">
         <v>514</v>
       </c>
     </row>
@@ -6610,22 +6625,22 @@
       <c r="A8" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="K8" s="65">
+      <c r="K8" s="66">
         <v>6.0</v>
       </c>
-      <c r="L8" s="65" t="s">
+      <c r="L8" s="66" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6633,13 +6648,13 @@
       <c r="A9" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="38" t="s">
         <v>519</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -6648,10 +6663,10 @@
       <c r="G9" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K9" s="65" t="s">
+      <c r="K9" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L9" s="65" t="s">
+      <c r="L9" s="66" t="s">
         <v>521</v>
       </c>
     </row>
@@ -6659,22 +6674,22 @@
       <c r="A10" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>523</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="K10" s="65">
+      <c r="K10" s="66">
         <v>6.0</v>
       </c>
-      <c r="L10" s="65" t="s">
+      <c r="L10" s="66" t="s">
         <v>39</v>
       </c>
     </row>
@@ -6682,13 +6697,13 @@
       <c r="A11" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="38" t="s">
         <v>526</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -6697,10 +6712,10 @@
       <c r="G11" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L11" s="65" t="s">
+      <c r="L11" s="66" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6708,19 +6723,19 @@
       <c r="A12" s="5" t="s">
         <v>529</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="38" t="s">
         <v>530</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="K12" s="65">
+      <c r="K12" s="66">
         <v>6.0</v>
       </c>
       <c r="L12" s="5" t="s">
@@ -6731,13 +6746,13 @@
       <c r="A13" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="38" t="s">
         <v>533</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -6746,10 +6761,10 @@
       <c r="G13" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K13" s="65" t="s">
+      <c r="K13" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L13" s="65" t="s">
+      <c r="L13" s="66" t="s">
         <v>535</v>
       </c>
     </row>
@@ -6757,22 +6772,22 @@
       <c r="A14" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="38" t="s">
         <v>537</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="K14" s="65">
+      <c r="K14" s="66">
         <v>6.0</v>
       </c>
-      <c r="L14" s="65" t="s">
+      <c r="L14" s="66" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6780,13 +6795,13 @@
       <c r="A15" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="38" t="s">
         <v>540</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E15" s="51" t="s">
+      <c r="E15" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -6795,10 +6810,10 @@
       <c r="G15" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K15" s="65" t="s">
+      <c r="K15" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L15" s="65" t="s">
+      <c r="L15" s="66" t="s">
         <v>542</v>
       </c>
     </row>
@@ -6806,22 +6821,22 @@
       <c r="A16" s="5" t="s">
         <v>543</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="38" t="s">
         <v>544</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="K16" s="65">
+      <c r="K16" s="66">
         <v>6.0</v>
       </c>
-      <c r="L16" s="65" t="s">
+      <c r="L16" s="66" t="s">
         <v>51</v>
       </c>
     </row>
@@ -6829,13 +6844,13 @@
       <c r="A17" s="5" t="s">
         <v>546</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="38" t="s">
         <v>547</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -6844,10 +6859,10 @@
       <c r="G17" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K17" s="65" t="s">
+      <c r="K17" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L17" s="65" t="s">
+      <c r="L17" s="66" t="s">
         <v>549</v>
       </c>
     </row>
@@ -6855,22 +6870,22 @@
       <c r="A18" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="38" t="s">
         <v>551</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="K18" s="65">
+      <c r="K18" s="66">
         <v>6.0</v>
       </c>
-      <c r="L18" s="65" t="s">
+      <c r="L18" s="66" t="s">
         <v>55</v>
       </c>
     </row>
@@ -6878,13 +6893,13 @@
       <c r="A19" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="38" t="s">
         <v>554</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F19" s="5" t="s">
@@ -6893,10 +6908,10 @@
       <c r="G19" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K19" s="65" t="s">
+      <c r="K19" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L19" s="65" t="s">
+      <c r="L19" s="66" t="s">
         <v>556</v>
       </c>
     </row>
@@ -6904,22 +6919,22 @@
       <c r="A20" s="5" t="s">
         <v>557</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="38" t="s">
         <v>558</v>
       </c>
-      <c r="C20" s="63" t="s">
+      <c r="C20" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E20" s="51" t="s">
+      <c r="E20" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="K20" s="65">
+      <c r="K20" s="66">
         <v>6.0</v>
       </c>
-      <c r="L20" s="65" t="s">
+      <c r="L20" s="66" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6927,13 +6942,13 @@
       <c r="A21" s="5" t="s">
         <v>560</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="38" t="s">
         <v>561</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E21" s="51" t="s">
+      <c r="E21" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -6942,153 +6957,153 @@
       <c r="G21" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K21" s="65" t="s">
+      <c r="K21" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L21" s="65" t="s">
+      <c r="L21" s="66" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="67" t="s">
         <v>564</v>
       </c>
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="68" t="s">
         <v>565</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="69" t="s">
         <v>492</v>
       </c>
-      <c r="D22" s="69"/>
-      <c r="E22" s="70" t="s">
+      <c r="D22" s="70"/>
+      <c r="E22" s="71" t="s">
         <v>449</v>
       </c>
-      <c r="F22" s="66" t="s">
+      <c r="F22" s="67" t="s">
         <v>566</v>
       </c>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="66">
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="67">
         <v>6.0</v>
       </c>
-      <c r="L22" s="66" t="s">
+      <c r="L22" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="M22" s="69"/>
+      <c r="M22" s="70"/>
     </row>
     <row r="23">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="67" t="s">
         <v>567</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="68" t="s">
         <v>568</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="69" t="s">
         <v>496</v>
       </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70" t="s">
+      <c r="D23" s="70"/>
+      <c r="E23" s="71" t="s">
         <v>446</v>
       </c>
-      <c r="F23" s="66" t="s">
+      <c r="F23" s="67" t="s">
         <v>569</v>
       </c>
-      <c r="G23" s="66" t="s">
+      <c r="G23" s="67" t="s">
         <v>498</v>
       </c>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="66" t="s">
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="67" t="s">
         <v>499</v>
       </c>
-      <c r="L23" s="66" t="s">
+      <c r="L23" s="67" t="s">
         <v>570</v>
       </c>
-      <c r="M23" s="69"/>
+      <c r="M23" s="70"/>
     </row>
     <row r="24">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="67" t="s">
         <v>571</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="68" t="s">
         <v>572</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="69" t="s">
         <v>492</v>
       </c>
-      <c r="D24" s="69"/>
-      <c r="E24" s="70" t="s">
+      <c r="D24" s="70"/>
+      <c r="E24" s="71" t="s">
         <v>449</v>
       </c>
-      <c r="F24" s="66" t="s">
+      <c r="F24" s="67" t="s">
         <v>573</v>
       </c>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="66">
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67">
         <v>6.0</v>
       </c>
-      <c r="L24" s="66" t="s">
+      <c r="L24" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="M24" s="69"/>
+      <c r="M24" s="70"/>
     </row>
     <row r="25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="67" t="s">
         <v>574</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="68" t="s">
         <v>575</v>
       </c>
-      <c r="C25" s="68" t="s">
+      <c r="C25" s="69" t="s">
         <v>496</v>
       </c>
-      <c r="D25" s="69"/>
-      <c r="E25" s="70" t="s">
+      <c r="D25" s="70"/>
+      <c r="E25" s="71" t="s">
         <v>446</v>
       </c>
-      <c r="F25" s="66" t="s">
+      <c r="F25" s="67" t="s">
         <v>576</v>
       </c>
-      <c r="G25" s="66" t="s">
+      <c r="G25" s="67" t="s">
         <v>498</v>
       </c>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="66" t="s">
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="67" t="s">
         <v>499</v>
       </c>
-      <c r="L25" s="66" t="s">
+      <c r="L25" s="67" t="s">
         <v>577</v>
       </c>
-      <c r="M25" s="69"/>
+      <c r="M25" s="70"/>
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="38" t="s">
         <v>579</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="K26" s="65">
+      <c r="K26" s="66">
         <v>6.0</v>
       </c>
-      <c r="L26" s="65" t="s">
+      <c r="L26" s="66" t="s">
         <v>71</v>
       </c>
     </row>
@@ -7096,13 +7111,13 @@
       <c r="A27" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="38" t="s">
         <v>582</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E27" s="51" t="s">
+      <c r="E27" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -7111,10 +7126,10 @@
       <c r="G27" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K27" s="65" t="s">
+      <c r="K27" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L27" s="65" t="s">
+      <c r="L27" s="66" t="s">
         <v>584</v>
       </c>
     </row>
@@ -7122,22 +7137,22 @@
       <c r="A28" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="38" t="s">
         <v>586</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E28" s="51" t="s">
+      <c r="E28" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="K28" s="65">
+      <c r="K28" s="66">
         <v>6.0</v>
       </c>
-      <c r="L28" s="65" t="s">
+      <c r="L28" s="66" t="s">
         <v>75</v>
       </c>
     </row>
@@ -7145,13 +7160,13 @@
       <c r="A29" s="5" t="s">
         <v>588</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="38" t="s">
         <v>589</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E29" s="51" t="s">
+      <c r="E29" s="52" t="s">
         <v>446</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -7160,10 +7175,10 @@
       <c r="G29" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="K29" s="65" t="s">
+      <c r="K29" s="66" t="s">
         <v>499</v>
       </c>
-      <c r="L29" s="65" t="s">
+      <c r="L29" s="66" t="s">
         <v>591</v>
       </c>
     </row>
@@ -7171,13 +7186,13 @@
       <c r="A30" s="5" t="s">
         <v>592</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="38" t="s">
         <v>593</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="52" t="s">
         <v>442</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -7186,208 +7201,208 @@
       <c r="G30" s="5" t="s">
         <v>594</v>
       </c>
-      <c r="K30" s="66" t="s">
+      <c r="K30" s="67" t="s">
         <v>595</v>
       </c>
-      <c r="L30" s="71" t="s">
+      <c r="L30" s="72" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="40" t="s">
         <v>598</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="73" t="s">
         <v>492</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="73" t="s">
+      <c r="D31" s="42"/>
+      <c r="E31" s="74" t="s">
         <v>449</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="41" t="s">
         <v>599</v>
       </c>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="40">
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="41">
         <v>0.0</v>
       </c>
-      <c r="L31" s="40" t="s">
+      <c r="L31" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="M31" s="41"/>
+      <c r="M31" s="42"/>
     </row>
     <row r="32">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="41" t="s">
         <v>600</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="40" t="s">
         <v>601</v>
       </c>
-      <c r="C32" s="72" t="s">
+      <c r="C32" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="73" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="74" t="s">
         <v>446</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="41" t="s">
         <v>602</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="66" t="s">
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="67" t="s">
         <v>604</v>
       </c>
-      <c r="L32" s="40" t="s">
+      <c r="L32" s="41" t="s">
         <v>605</v>
       </c>
-      <c r="M32" s="41"/>
+      <c r="M32" s="42"/>
     </row>
     <row r="33">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="41" t="s">
         <v>606</v>
       </c>
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="73" t="s">
+      <c r="D33" s="42"/>
+      <c r="E33" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F33" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="41" t="s">
         <v>608</v>
       </c>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="66" t="s">
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="67" t="s">
         <v>595</v>
       </c>
-      <c r="L33" s="40" t="s">
+      <c r="L33" s="41" t="s">
         <v>609</v>
       </c>
-      <c r="M33" s="41"/>
+      <c r="M33" s="42"/>
     </row>
     <row r="34">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="41" t="s">
         <v>610</v>
       </c>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="40" t="s">
         <v>611</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="73" t="s">
+      <c r="D34" s="42"/>
+      <c r="E34" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="G34" s="40" t="s">
+      <c r="G34" s="41" t="s">
         <v>612</v>
       </c>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="66" t="s">
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="67" t="s">
         <v>595</v>
       </c>
-      <c r="L34" s="40" t="s">
+      <c r="L34" s="41" t="s">
         <v>613</v>
       </c>
-      <c r="M34" s="41"/>
+      <c r="M34" s="42"/>
     </row>
     <row r="35">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="41" t="s">
         <v>614</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="40" t="s">
         <v>615</v>
       </c>
-      <c r="C35" s="72" t="s">
+      <c r="C35" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="73" t="s">
+      <c r="D35" s="42"/>
+      <c r="E35" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="G35" s="40" t="s">
+      <c r="G35" s="41" t="s">
         <v>616</v>
       </c>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="66" t="s">
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="67" t="s">
         <v>595</v>
       </c>
-      <c r="L35" s="40" t="s">
+      <c r="L35" s="41" t="s">
         <v>617</v>
       </c>
-      <c r="M35" s="41"/>
+      <c r="M35" s="42"/>
     </row>
     <row r="36">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="41" t="s">
         <v>618</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B36" s="40" t="s">
         <v>619</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="73" t="s">
+      <c r="D36" s="42"/>
+      <c r="E36" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" s="41" t="s">
         <v>603</v>
       </c>
-      <c r="G36" s="40" t="s">
+      <c r="G36" s="41" t="s">
         <v>620</v>
       </c>
-      <c r="H36" s="41"/>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="66" t="s">
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="67" t="s">
         <v>595</v>
       </c>
-      <c r="L36" s="40" t="s">
+      <c r="L36" s="41" t="s">
         <v>621</v>
       </c>
-      <c r="M36" s="41"/>
+      <c r="M36" s="42"/>
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="38" t="s">
         <v>623</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -7404,13 +7419,13 @@
       <c r="A38" s="5" t="s">
         <v>625</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="38" t="s">
         <v>626</v>
       </c>
-      <c r="C38" s="63" t="s">
+      <c r="C38" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="52" t="s">
         <v>442</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -7419,7 +7434,7 @@
       <c r="G38" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="K38" s="66" t="s">
+      <c r="K38" s="67" t="s">
         <v>629</v>
       </c>
       <c r="L38" s="5" t="s">
@@ -7427,76 +7442,76 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="41" t="s">
         <v>631</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="40" t="s">
         <v>632</v>
       </c>
-      <c r="C39" s="72" t="s">
+      <c r="C39" s="73" t="s">
         <v>492</v>
       </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="73" t="s">
+      <c r="D39" s="42"/>
+      <c r="E39" s="74" t="s">
         <v>449</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="41" t="s">
         <v>633</v>
       </c>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="40">
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="41">
         <v>0.0</v>
       </c>
-      <c r="L39" s="40" t="s">
+      <c r="L39" s="41" t="s">
         <v>396</v>
       </c>
-      <c r="M39" s="41"/>
+      <c r="M39" s="42"/>
     </row>
     <row r="40">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="41" t="s">
         <v>634</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="40" t="s">
         <v>635</v>
       </c>
-      <c r="C40" s="72" t="s">
+      <c r="C40" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="73" t="s">
+      <c r="D40" s="42"/>
+      <c r="E40" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" s="41" t="s">
         <v>636</v>
       </c>
-      <c r="G40" s="40" t="s">
+      <c r="G40" s="41" t="s">
         <v>637</v>
       </c>
-      <c r="H40" s="41"/>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="66" t="s">
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="67" t="s">
         <v>629</v>
       </c>
-      <c r="L40" s="40" t="s">
+      <c r="L40" s="41" t="s">
         <v>638</v>
       </c>
-      <c r="M40" s="41"/>
+      <c r="M40" s="42"/>
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="38" t="s">
         <v>640</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="64" t="s">
         <v>492</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="52" t="s">
         <v>449</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -7513,13 +7528,13 @@
       <c r="A42" s="5" t="s">
         <v>642</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="38" t="s">
         <v>643</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="64" t="s">
         <v>496</v>
       </c>
-      <c r="E42" s="51" t="s">
+      <c r="E42" s="52" t="s">
         <v>442</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -7528,7 +7543,7 @@
       <c r="G42" s="5" t="s">
         <v>645</v>
       </c>
-      <c r="K42" s="66" t="s">
+      <c r="K42" s="67" t="s">
         <v>629</v>
       </c>
       <c r="L42" s="5" t="s">
@@ -7536,79 +7551,79 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="41" t="s">
         <v>647</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="40" t="s">
         <v>648</v>
       </c>
-      <c r="C43" s="72" t="s">
+      <c r="C43" s="73" t="s">
         <v>492</v>
       </c>
-      <c r="D43" s="41"/>
-      <c r="E43" s="73" t="s">
+      <c r="D43" s="42"/>
+      <c r="E43" s="74" t="s">
         <v>449</v>
       </c>
-      <c r="F43" s="40" t="s">
+      <c r="F43" s="41" t="s">
         <v>649</v>
       </c>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="40">
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="41">
         <v>0.0</v>
       </c>
-      <c r="L43" s="40" t="s">
+      <c r="L43" s="41" t="s">
         <v>404</v>
       </c>
-      <c r="M43" s="41"/>
+      <c r="M43" s="42"/>
     </row>
     <row r="44">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="41" t="s">
         <v>650</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="40" t="s">
         <v>651</v>
       </c>
-      <c r="C44" s="72" t="s">
+      <c r="C44" s="73" t="s">
         <v>496</v>
       </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="73" t="s">
+      <c r="D44" s="42"/>
+      <c r="E44" s="74" t="s">
         <v>442</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="41" t="s">
         <v>652</v>
       </c>
-      <c r="G44" s="40" t="s">
+      <c r="G44" s="41" t="s">
         <v>653</v>
       </c>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="66" t="s">
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="67" t="s">
         <v>629</v>
       </c>
-      <c r="L44" s="40" t="s">
+      <c r="L44" s="41" t="s">
         <v>654</v>
       </c>
-      <c r="M44" s="41"/>
+      <c r="M44" s="42"/>
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="38" t="s">
         <v>656</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="D45" s="74" t="s">
+      <c r="D45" s="75" t="s">
         <v>658</v>
       </c>
-      <c r="E45" s="50"/>
+      <c r="E45" s="51"/>
       <c r="F45" s="5" t="s">
         <v>659</v>
       </c>
@@ -7656,10 +7671,10 @@
       <c r="E1" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="61" t="s">
         <v>489</v>
       </c>
     </row>
@@ -8009,245 +8024,245 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="80" t="s">
         <v>683</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="78" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="81" t="s">
         <v>684</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>685</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="82" t="s">
         <v>686</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="81" t="s">
         <v>687</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>688</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="82" t="s">
         <v>689</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="81" t="s">
         <v>690</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>691</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="82" t="s">
         <v>692</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
     <row r="5">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="81" t="s">
         <v>693</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="82" t="s">
         <v>695</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="81" t="s">
         <v>696</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>697</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="82" t="s">
         <v>698</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
     </row>
     <row r="7">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="81" t="s">
         <v>699</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>700</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="82" t="s">
         <v>701</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="81" t="s">
         <v>702</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>703</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="82" t="s">
         <v>704</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="80" t="s">
+      <c r="A9" s="81" t="s">
         <v>705</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>706</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="82" t="s">
         <v>707</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="81" t="s">
         <v>708</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>709</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="82" t="s">
         <v>710</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="81" t="s">
         <v>711</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>712</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="82" t="s">
         <v>713</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="81" t="s">
         <v>714</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>715</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="82" t="s">
         <v>716</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="81" t="s">
         <v>717</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>718</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>719</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="81" t="s">
         <v>720</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>721</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="82" t="s">
         <v>722</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="81" t="s">
         <v>723</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>724</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="82" t="s">
         <v>725</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="81" t="s">
         <v>726</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>727</v>
       </c>
-      <c r="C16" s="81" t="s">
+      <c r="C16" s="82" t="s">
         <v>728</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
     </row>
     <row r="17">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="81" t="s">
         <v>729</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>730</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="82" t="s">
         <v>698</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="80" t="s">
+      <c r="A18" s="81" t="s">
         <v>731</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>732</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="82" t="s">
         <v>733</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="81" t="s">
         <v>734</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -8256,39 +8271,39 @@
       <c r="C19" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="84" t="s">
         <v>737</v>
       </c>
       <c r="E19" s="17"/>
     </row>
     <row r="20">
-      <c r="A20" s="80" t="s">
+      <c r="A20" s="81" t="s">
         <v>738</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>739</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="85" t="s">
         <v>740</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
     </row>
     <row r="21">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="81" t="s">
         <v>741</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>742</v>
       </c>
-      <c r="C21" s="84" t="s">
+      <c r="C21" s="85" t="s">
         <v>743</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="81" t="s">
         <v>744</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -8297,272 +8312,272 @@
       <c r="C22" s="31" t="s">
         <v>736</v>
       </c>
-      <c r="D22" s="84" t="s">
+      <c r="D22" s="85" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="81" t="s">
         <v>747</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>748</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="82" t="s">
         <v>749</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
     </row>
     <row r="24">
-      <c r="A24" s="80" t="s">
+      <c r="A24" s="81" t="s">
         <v>750</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>751</v>
       </c>
-      <c r="C24" s="85" t="s">
+      <c r="C24" s="86" t="s">
         <v>752</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
     <row r="25">
-      <c r="A25" s="86" t="s">
+      <c r="A25" s="87" t="s">
         <v>753</v>
       </c>
-      <c r="B25" s="87" t="s">
+      <c r="B25" s="88" t="s">
         <v>754</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="89" t="s">
         <v>755</v>
       </c>
-      <c r="D25" s="89"/>
-      <c r="E25" s="89"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
     </row>
     <row r="26">
-      <c r="A26" s="80" t="s">
+      <c r="A26" s="81" t="s">
         <v>756</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>757</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="C26" s="82" t="s">
         <v>758</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
     <row r="27">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="81" t="s">
         <v>759</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>760</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="82" t="s">
         <v>761</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
     <row r="28">
-      <c r="A28" s="80" t="s">
+      <c r="A28" s="81" t="s">
         <v>762</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>763</v>
       </c>
-      <c r="C28" s="81" t="s">
+      <c r="C28" s="82" t="s">
         <v>764</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
     <row r="29">
-      <c r="A29" s="80" t="s">
+      <c r="A29" s="81" t="s">
         <v>765</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>766</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="82" t="s">
         <v>767</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
     </row>
     <row r="30">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="81" t="s">
         <v>768</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>769</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="82" t="s">
         <v>770</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="81" t="s">
         <v>771</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>772</v>
       </c>
-      <c r="C31" s="81" t="s">
+      <c r="C31" s="82" t="s">
         <v>773</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
     <row r="32">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="81" t="s">
         <v>774</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>775</v>
       </c>
-      <c r="C32" s="81" t="s">
+      <c r="C32" s="82" t="s">
         <v>776</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
     <row r="33">
-      <c r="A33" s="80" t="s">
+      <c r="A33" s="81" t="s">
         <v>777</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>778</v>
       </c>
-      <c r="C33" s="81" t="s">
+      <c r="C33" s="82" t="s">
         <v>779</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
     <row r="34">
-      <c r="A34" s="80" t="s">
+      <c r="A34" s="81" t="s">
         <v>780</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>781</v>
       </c>
-      <c r="C34" s="81" t="s">
+      <c r="C34" s="82" t="s">
         <v>782</v>
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
     <row r="35">
-      <c r="A35" s="80" t="s">
+      <c r="A35" s="81" t="s">
         <v>783</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>784</v>
       </c>
-      <c r="C35" s="81" t="s">
+      <c r="C35" s="82" t="s">
         <v>785</v>
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
     <row r="36">
-      <c r="A36" s="80" t="s">
+      <c r="A36" s="81" t="s">
         <v>786</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>787</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C36" s="91" t="s">
         <v>788</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
     </row>
     <row r="37">
-      <c r="A37" s="80" t="s">
+      <c r="A37" s="81" t="s">
         <v>789</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>790</v>
       </c>
-      <c r="C37" s="90" t="s">
+      <c r="C37" s="91" t="s">
         <v>791</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
     </row>
     <row r="38">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="81" t="s">
         <v>792</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>793</v>
       </c>
-      <c r="C38" s="90" t="s">
+      <c r="C38" s="91" t="s">
         <v>794</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
     </row>
     <row r="39">
-      <c r="A39" s="80" t="s">
+      <c r="A39" s="81" t="s">
         <v>795</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>688</v>
       </c>
-      <c r="C39" s="84" t="s">
+      <c r="C39" s="85" t="s">
         <v>796</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
     </row>
     <row r="40">
-      <c r="A40" s="80" t="s">
+      <c r="A40" s="81" t="s">
         <v>797</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>798</v>
       </c>
-      <c r="C40" s="84" t="s">
+      <c r="C40" s="85" t="s">
         <v>799</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
     </row>
     <row r="41">
-      <c r="A41" s="80" t="s">
+      <c r="A41" s="81" t="s">
         <v>800</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>801</v>
       </c>
-      <c r="C41" s="91" t="s">
+      <c r="C41" s="92" t="s">
         <v>802</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
     </row>
     <row r="42">
-      <c r="A42" s="80" t="s">
+      <c r="A42" s="81" t="s">
         <v>803</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>804</v>
       </c>
-      <c r="C42" s="92" t="s">
+      <c r="C42" s="93" t="s">
         <v>805</v>
       </c>
-      <c r="D42" s="93"/>
-      <c r="E42" s="93"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
     </row>
     <row r="43">
-      <c r="A43" s="80" t="s">
+      <c r="A43" s="81" t="s">
         <v>806</v>
       </c>
       <c r="B43" s="11" t="s">
@@ -8573,7 +8588,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="80" t="s">
+      <c r="A44" s="81" t="s">
         <v>809</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -8584,7 +8599,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="80" t="s">
+      <c r="A45" s="81" t="s">
         <v>812</v>
       </c>
       <c r="B45" s="4" t="s">
@@ -8595,7 +8610,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="80" t="s">
+      <c r="A46" s="81" t="s">
         <v>815</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -8604,10 +8619,10 @@
       <c r="C46" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="E46" s="94"/>
+      <c r="E46" s="95"/>
     </row>
     <row r="47">
-      <c r="A47" s="80" t="s">
+      <c r="A47" s="81" t="s">
         <v>818</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -8616,42 +8631,42 @@
       <c r="C47" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="E47" s="94"/>
+      <c r="E47" s="95"/>
     </row>
     <row r="48">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="81" t="s">
         <v>821</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="C48" s="95" t="s">
+      <c r="C48" s="96" t="s">
         <v>823</v>
       </c>
-      <c r="D48" s="94"/>
-      <c r="E48" s="94"/>
+      <c r="D48" s="95"/>
+      <c r="E48" s="95"/>
     </row>
     <row r="49">
-      <c r="A49" s="80" t="s">
+      <c r="A49" s="81" t="s">
         <v>824</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>825</v>
       </c>
-      <c r="C49" s="96" t="s">
+      <c r="C49" s="97" t="s">
         <v>826</v>
       </c>
-      <c r="D49" s="94"/>
-      <c r="E49" s="94"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="95"/>
     </row>
     <row r="50">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="81" t="s">
         <v>827</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>828</v>
       </c>
-      <c r="C50" s="96" t="s">
+      <c r="C50" s="97" t="s">
         <v>829</v>
       </c>
     </row>
@@ -8677,7 +8692,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -8794,28 +8809,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="63" t="s">
         <v>481</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>834</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="63" t="s">
         <v>835</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>836</v>
       </c>
-      <c r="H1" s="98" t="s">
+      <c r="H1" s="99" t="s">
         <v>489</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -8832,11 +8847,11 @@
       <c r="C2" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="F2" s="74"/>
+      <c r="F2" s="75"/>
       <c r="H2" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="I2" s="99" t="s">
+      <c r="I2" s="100" t="s">
         <v>841</v>
       </c>
     </row>
@@ -8850,7 +8865,7 @@
       <c r="C3" s="5" t="s">
         <v>843</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="75"/>
       <c r="H3" s="5" t="s">
         <v>844</v>
       </c>
@@ -8868,7 +8883,7 @@
       <c r="C4" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="75"/>
       <c r="H4" s="5" t="s">
         <v>844</v>
       </c>
@@ -8886,7 +8901,7 @@
       <c r="C5" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="F5" s="74"/>
+      <c r="F5" s="75"/>
       <c r="H5" s="5" t="s">
         <v>844</v>
       </c>
@@ -8904,7 +8919,7 @@
       <c r="C6" s="5" t="s">
         <v>852</v>
       </c>
-      <c r="F6" s="74"/>
+      <c r="F6" s="75"/>
       <c r="H6" s="5" t="s">
         <v>844</v>
       </c>
@@ -8922,7 +8937,7 @@
       <c r="C7" s="5" t="s">
         <v>854</v>
       </c>
-      <c r="F7" s="74"/>
+      <c r="F7" s="75"/>
       <c r="H7" s="5" t="s">
         <v>844</v>
       </c>
@@ -9136,7 +9151,7 @@
       <c r="A12" s="11" t="s">
         <v>872</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="101" t="s">
         <v>873</v>
       </c>
       <c r="C12" s="11"/>
@@ -9153,7 +9168,7 @@
       <c r="A13" s="11" t="s">
         <v>874</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="101" t="s">
         <v>875</v>
       </c>
       <c r="C13" s="11"/>
@@ -9183,7 +9198,7 @@
       <c r="A15" s="11" t="s">
         <v>876</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="100" t="s">
         <v>877</v>
       </c>
       <c r="C15" s="11"/>
@@ -9200,24 +9215,24 @@
       <c r="A16" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="101"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="101"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="101"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
     </row>
     <row r="17">
       <c r="A17" s="11" t="s">
         <v>879</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="99" t="s">
         <v>880</v>
       </c>
     </row>
@@ -9240,37 +9255,37 @@
       <c r="A23" s="11"/>
     </row>
     <row r="24">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="102" t="s">
         <v>881</v>
       </c>
-      <c r="B24" s="102" t="s">
+      <c r="B24" s="103" t="s">
         <v>882</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="102" t="s">
         <v>883</v>
       </c>
-      <c r="B25" s="102" t="s">
+      <c r="B25" s="103" t="s">
         <v>884</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="101" t="s">
+      <c r="A26" s="102" t="s">
         <v>885</v>
       </c>
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="104" t="s">
         <v>886</v>
       </c>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="104"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
-      <c r="K26" s="104"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="105"/>
+      <c r="K26" s="105"/>
     </row>
     <row r="27" hidden="1">
       <c r="A27" s="11" t="s">
@@ -9317,7 +9332,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -9334,7 +9349,7 @@
       <c r="A2" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="107" t="s">
         <v>892</v>
       </c>
     </row>
@@ -9342,7 +9357,7 @@
       <c r="A3" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="C3" s="106" t="s">
+      <c r="C3" s="107" t="s">
         <v>894</v>
       </c>
     </row>
@@ -9350,7 +9365,7 @@
       <c r="A4" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="107" t="s">
         <v>896</v>
       </c>
     </row>
@@ -9358,7 +9373,7 @@
       <c r="A5" s="5" t="s">
         <v>897</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="108" t="s">
         <v>898</v>
       </c>
     </row>
@@ -9366,20 +9381,23 @@
       <c r="A6" s="5" t="s">
         <v>844</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="109" t="s">
         <v>899</v>
       </c>
-      <c r="D6" s="108"/>
+      <c r="D6" s="110"/>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
         <v>900</v>
       </c>
-      <c r="C7" s="107" t="s">
+      <c r="C7" s="109" t="s">
         <v>901</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="C5"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>